<commit_message>
Aggiornato il file report all'ultima versione
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-RAP/V.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-RAP/V.2.0/report-checklist.xlsx
@@ -11,7 +11,7 @@
     <sheet state="hidden" name="Sheet1" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">TestCases!$A$9:$W$191</definedName>
+    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">TestCases!$A$9:$W$192</definedName>
     <definedName hidden="1" localSheetId="4" name="_xlnm._FilterDatabase">Summary!$A$1:$G$10</definedName>
   </definedNames>
   <calcPr/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="474">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -53,7 +53,7 @@
     <t>2) Per tutti i casi di test coerenti con la/e tipologia/e di documento utilizzata/e dal software è necessario compilare SEMPRE la colonna APPLICABILITA' con SI o NO</t>
   </si>
   <si>
-    <t>3) Nel caso in cui tra le tipologie documentali oggetto di accreditamento per l'applicativo figurino PSS, RAP, RAD, RSA, LDO, LAB, VPS, SING_VACC, CERT_VACC i relativi casi di test con id 444, 417, 418, 460, 446, 448, 450, 452,454, 456, 457, 458 che recepiscono quanto previsto dal Decreto 07 settembre 2023, devono essere obbligatoriamente eseguiti e compilati (la colonna APPLICABILITA' deve essere valorizzata con SI)</t>
+    <t>3) Nel caso in cui tra le tipologie documentali oggetto di accreditamento per l'applicativo figurino PSS, RAP, RAD, RSA, LDO, LAB, VPS, SING_VACC, CERT_VACC i relativi casi di test con id 444, 417, 418, 460, 448, 450, 452,454, 456, 457, 458, 471 che recepiscono quanto previsto dal Decreto 07 settembre 2023, devono essere obbligatoriamente eseguiti e compilati (la colonna APPLICABILITA' deve essere valorizzata con SI)</t>
   </si>
   <si>
     <t>4) Se il test è applicabile la colonna APPLICABILITA' deve essere compilata con SI e dovranno essere valorizzate:
@@ -167,13 +167,13 @@
     <t>IDENTIFICATIVI SOFTWARE</t>
   </si>
   <si>
-    <t>subject_application_id: WLEXT-RAP</t>
-  </si>
-  <si>
-    <t>subject_application_vendor: GESAN SRL</t>
-  </si>
-  <si>
-    <t>subject_application_version: 2.0</t>
+    <t>subject_application_id:</t>
+  </si>
+  <si>
+    <t>subject_application_vendor:</t>
+  </si>
+  <si>
+    <t>subject_application_version:</t>
   </si>
   <si>
     <t>ID</t>
@@ -1037,6 +1037,13 @@
     <t>VALIDAZIONE_VPS_TIMEOUT</t>
   </si>
   <si>
+    <t>VALIDAZIONE_CDA2_LAB_CT7_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT9_KO</t>
   </si>
   <si>
@@ -1058,13 +1065,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>VALIDAZIONE_CDA2_LAB_CT12_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT13_KO</t>
   </si>
   <si>
@@ -1198,13 +1198,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>VALIDAZIONE_CDA2_RAD_CT12_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.  
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RAD_CT13_KO</t>
   </si>
   <si>
@@ -1637,13 +1630,6 @@
   <si>
     <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RSA_CT12_KO</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT13_KO</t>
@@ -2116,20 +2102,6 @@
 </t>
   </si>
   <si>
-    <t>VALIDAZIONE_CDA2_RAD_CT1</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
-Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_RAD_CT2</t>
-  </si>
-  <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
-Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RSA_CT24</t>
   </si>
   <si>
@@ -2263,7 +2235,7 @@
   </si>
   <si>
     <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test SING_VACC" e "CDA2_Scheda_Singola Vaccinazione_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO.xlsx" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT19_KO</t>
@@ -2294,6 +2266,41 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 25" riportata nei documenti "casi di test RAP" e "CDA2_Referto_di_Anatomia_Patologica_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT25</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT26</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 26" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LAB_CT19_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT27_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.  
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 27" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT28_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 28" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
     <t>Razionale di Applicabilità</t>
   </si>
   <si>
@@ -2321,7 +2328,7 @@
     <t>Versione:</t>
   </si>
   <si>
-    <t>8.2.4</t>
+    <t>8.2.6</t>
   </si>
   <si>
     <t>Validazione</t>
@@ -2330,7 +2337,7 @@
     <t>4, 452</t>
   </si>
   <si>
-    <t>28,36,44,53,55,56,57,58,59,60,61,62, 466</t>
+    <t>28,36,44,53,55,56,57,59,60,61,62, 466, 473</t>
   </si>
   <si>
     <t>450, 451</t>
@@ -2339,7 +2346,10 @@
     <t>29,37,45,64,66,67,68,69,70,71,72,73,74, 467</t>
   </si>
   <si>
-    <t>31,39,47,76,78,79,80,81,82,83,84,85,86,87,88,89,90,91,92,93, 462</t>
+    <t>471, 472</t>
+  </si>
+  <si>
+    <t>31,39,47,76,78,79,80,81,83,84,85,86,87,88,89,90,91,92,93, 462, 474</t>
   </si>
   <si>
     <t>458, 459</t>
@@ -2363,7 +2373,7 @@
     <t>448, 449</t>
   </si>
   <si>
-    <t>32,40,48,152,154,155,156,157,158,159,160,161,162,163,164,165,166,167,168,169, 461, 468</t>
+    <t>32,40,48,152,154,155,156,157,159,160,161,162,163,164,165,166,167,168,169, 461, 468, 475</t>
   </si>
   <si>
     <t>444, 445</t>
@@ -2740,7 +2750,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="64">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2792,7 +2802,7 @@
     </xf>
     <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -2824,7 +2834,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="19" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -2848,22 +2858,33 @@
       <alignment horizontal="center" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="22" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="21" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="21" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="21" fillId="0" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf borderId="21" fillId="0" fontId="2" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="22" fillId="0" fontId="2" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="21" fillId="0" fontId="2" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="23" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -6552,7 +6573,7 @@
     </row>
     <row r="35" ht="10.5" hidden="1" customHeight="1">
       <c r="A35" s="33">
-        <v>55.0</v>
+        <v>53.0</v>
       </c>
       <c r="B35" s="33" t="s">
         <v>46</v>
@@ -6589,7 +6610,7 @@
     </row>
     <row r="36" ht="10.5" hidden="1" customHeight="1">
       <c r="A36" s="33">
-        <v>56.0</v>
+        <v>55.0</v>
       </c>
       <c r="B36" s="33" t="s">
         <v>46</v>
@@ -6626,7 +6647,7 @@
     </row>
     <row r="37" ht="10.5" hidden="1" customHeight="1">
       <c r="A37" s="33">
-        <v>57.0</v>
+        <v>56.0</v>
       </c>
       <c r="B37" s="33" t="s">
         <v>46</v>
@@ -6663,7 +6684,7 @@
     </row>
     <row r="38" ht="10.5" hidden="1" customHeight="1">
       <c r="A38" s="33">
-        <v>58.0</v>
+        <v>57.0</v>
       </c>
       <c r="B38" s="33" t="s">
         <v>46</v>
@@ -7403,7 +7424,7 @@
     </row>
     <row r="58" ht="10.5" hidden="1" customHeight="1">
       <c r="A58" s="33">
-        <v>82.0</v>
+        <v>83.0</v>
       </c>
       <c r="B58" s="33" t="s">
         <v>46</v>
@@ -7440,7 +7461,7 @@
     </row>
     <row r="59" ht="10.5" hidden="1" customHeight="1">
       <c r="A59" s="33">
-        <v>83.0</v>
+        <v>84.0</v>
       </c>
       <c r="B59" s="33" t="s">
         <v>46</v>
@@ -7477,7 +7498,7 @@
     </row>
     <row r="60" ht="10.5" hidden="1" customHeight="1">
       <c r="A60" s="33">
-        <v>84.0</v>
+        <v>85.0</v>
       </c>
       <c r="B60" s="33" t="s">
         <v>46</v>
@@ -7514,7 +7535,7 @@
     </row>
     <row r="61" ht="10.5" hidden="1" customHeight="1">
       <c r="A61" s="33">
-        <v>85.0</v>
+        <v>86.0</v>
       </c>
       <c r="B61" s="33" t="s">
         <v>46</v>
@@ -7551,7 +7572,7 @@
     </row>
     <row r="62" ht="10.5" hidden="1" customHeight="1">
       <c r="A62" s="33">
-        <v>86.0</v>
+        <v>87.0</v>
       </c>
       <c r="B62" s="33" t="s">
         <v>46</v>
@@ -7588,7 +7609,7 @@
     </row>
     <row r="63" ht="10.5" hidden="1" customHeight="1">
       <c r="A63" s="33">
-        <v>87.0</v>
+        <v>88.0</v>
       </c>
       <c r="B63" s="33" t="s">
         <v>46</v>
@@ -7625,7 +7646,7 @@
     </row>
     <row r="64" ht="10.5" hidden="1" customHeight="1">
       <c r="A64" s="33">
-        <v>88.0</v>
+        <v>89.0</v>
       </c>
       <c r="B64" s="33" t="s">
         <v>46</v>
@@ -7662,7 +7683,7 @@
     </row>
     <row r="65" ht="10.5" hidden="1" customHeight="1">
       <c r="A65" s="33">
-        <v>89.0</v>
+        <v>90.0</v>
       </c>
       <c r="B65" s="33" t="s">
         <v>46</v>
@@ -7699,7 +7720,7 @@
     </row>
     <row r="66" ht="10.5" hidden="1" customHeight="1">
       <c r="A66" s="33">
-        <v>90.0</v>
+        <v>91.0</v>
       </c>
       <c r="B66" s="33" t="s">
         <v>46</v>
@@ -7736,7 +7757,7 @@
     </row>
     <row r="67" ht="10.5" hidden="1" customHeight="1">
       <c r="A67" s="33">
-        <v>91.0</v>
+        <v>92.0</v>
       </c>
       <c r="B67" s="33" t="s">
         <v>46</v>
@@ -7773,7 +7794,7 @@
     </row>
     <row r="68" ht="10.5" hidden="1" customHeight="1">
       <c r="A68" s="33">
-        <v>92.0</v>
+        <v>93.0</v>
       </c>
       <c r="B68" s="33" t="s">
         <v>46</v>
@@ -7810,13 +7831,13 @@
     </row>
     <row r="69" ht="10.5" hidden="1" customHeight="1">
       <c r="A69" s="33">
-        <v>93.0</v>
+        <v>95.0</v>
       </c>
       <c r="B69" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C69" s="40" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D69" s="33" t="s">
         <v>169</v>
@@ -7847,7 +7868,7 @@
     </row>
     <row r="70" ht="10.5" hidden="1" customHeight="1">
       <c r="A70" s="33">
-        <v>95.0</v>
+        <v>97.0</v>
       </c>
       <c r="B70" s="33" t="s">
         <v>46</v>
@@ -7884,7 +7905,7 @@
     </row>
     <row r="71" ht="10.5" hidden="1" customHeight="1">
       <c r="A71" s="33">
-        <v>97.0</v>
+        <v>98.0</v>
       </c>
       <c r="B71" s="33" t="s">
         <v>46</v>
@@ -7921,7 +7942,7 @@
     </row>
     <row r="72" ht="10.5" hidden="1" customHeight="1">
       <c r="A72" s="33">
-        <v>98.0</v>
+        <v>99.0</v>
       </c>
       <c r="B72" s="33" t="s">
         <v>46</v>
@@ -7958,7 +7979,7 @@
     </row>
     <row r="73" ht="10.5" hidden="1" customHeight="1">
       <c r="A73" s="33">
-        <v>99.0</v>
+        <v>100.0</v>
       </c>
       <c r="B73" s="33" t="s">
         <v>46</v>
@@ -7995,7 +8016,7 @@
     </row>
     <row r="74" ht="10.5" hidden="1" customHeight="1">
       <c r="A74" s="33">
-        <v>100.0</v>
+        <v>101.0</v>
       </c>
       <c r="B74" s="33" t="s">
         <v>46</v>
@@ -8032,7 +8053,7 @@
     </row>
     <row r="75" ht="10.5" hidden="1" customHeight="1">
       <c r="A75" s="33">
-        <v>101.0</v>
+        <v>102.0</v>
       </c>
       <c r="B75" s="33" t="s">
         <v>46</v>
@@ -8069,7 +8090,7 @@
     </row>
     <row r="76" ht="10.5" hidden="1" customHeight="1">
       <c r="A76" s="33">
-        <v>102.0</v>
+        <v>103.0</v>
       </c>
       <c r="B76" s="33" t="s">
         <v>46</v>
@@ -8106,7 +8127,7 @@
     </row>
     <row r="77" ht="10.5" hidden="1" customHeight="1">
       <c r="A77" s="33">
-        <v>103.0</v>
+        <v>104.0</v>
       </c>
       <c r="B77" s="33" t="s">
         <v>46</v>
@@ -8143,7 +8164,7 @@
     </row>
     <row r="78" ht="10.5" hidden="1" customHeight="1">
       <c r="A78" s="33">
-        <v>104.0</v>
+        <v>105.0</v>
       </c>
       <c r="B78" s="33" t="s">
         <v>46</v>
@@ -8180,7 +8201,7 @@
     </row>
     <row r="79" ht="10.5" hidden="1" customHeight="1">
       <c r="A79" s="33">
-        <v>105.0</v>
+        <v>106.0</v>
       </c>
       <c r="B79" s="33" t="s">
         <v>46</v>
@@ -8217,13 +8238,13 @@
     </row>
     <row r="80" ht="10.5" hidden="1" customHeight="1">
       <c r="A80" s="33">
-        <v>106.0</v>
+        <v>108.0</v>
       </c>
       <c r="B80" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C80" s="40" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D80" s="33" t="s">
         <v>191</v>
@@ -8254,7 +8275,7 @@
     </row>
     <row r="81" ht="10.5" hidden="1" customHeight="1">
       <c r="A81" s="33">
-        <v>108.0</v>
+        <v>110.0</v>
       </c>
       <c r="B81" s="33" t="s">
         <v>46</v>
@@ -8291,7 +8312,7 @@
     </row>
     <row r="82" ht="10.5" hidden="1" customHeight="1">
       <c r="A82" s="33">
-        <v>110.0</v>
+        <v>111.0</v>
       </c>
       <c r="B82" s="33" t="s">
         <v>46</v>
@@ -8328,7 +8349,7 @@
     </row>
     <row r="83" ht="10.5" hidden="1" customHeight="1">
       <c r="A83" s="33">
-        <v>111.0</v>
+        <v>112.0</v>
       </c>
       <c r="B83" s="33" t="s">
         <v>46</v>
@@ -8365,7 +8386,7 @@
     </row>
     <row r="84" ht="10.5" hidden="1" customHeight="1">
       <c r="A84" s="33">
-        <v>112.0</v>
+        <v>113.0</v>
       </c>
       <c r="B84" s="33" t="s">
         <v>46</v>
@@ -8402,7 +8423,7 @@
     </row>
     <row r="85" ht="10.5" hidden="1" customHeight="1">
       <c r="A85" s="33">
-        <v>113.0</v>
+        <v>114.0</v>
       </c>
       <c r="B85" s="33" t="s">
         <v>46</v>
@@ -8439,7 +8460,7 @@
     </row>
     <row r="86" ht="10.5" hidden="1" customHeight="1">
       <c r="A86" s="33">
-        <v>114.0</v>
+        <v>115.0</v>
       </c>
       <c r="B86" s="33" t="s">
         <v>46</v>
@@ -8476,7 +8497,7 @@
     </row>
     <row r="87" ht="10.5" hidden="1" customHeight="1">
       <c r="A87" s="33">
-        <v>115.0</v>
+        <v>116.0</v>
       </c>
       <c r="B87" s="33" t="s">
         <v>46</v>
@@ -8513,7 +8534,7 @@
     </row>
     <row r="88" ht="10.5" hidden="1" customHeight="1">
       <c r="A88" s="33">
-        <v>116.0</v>
+        <v>117.0</v>
       </c>
       <c r="B88" s="33" t="s">
         <v>46</v>
@@ -8550,7 +8571,7 @@
     </row>
     <row r="89" ht="10.5" hidden="1" customHeight="1">
       <c r="A89" s="33">
-        <v>117.0</v>
+        <v>118.0</v>
       </c>
       <c r="B89" s="33" t="s">
         <v>46</v>
@@ -8587,7 +8608,7 @@
     </row>
     <row r="90" ht="10.5" hidden="1" customHeight="1">
       <c r="A90" s="33">
-        <v>118.0</v>
+        <v>119.0</v>
       </c>
       <c r="B90" s="33" t="s">
         <v>46</v>
@@ -8624,7 +8645,7 @@
     </row>
     <row r="91" ht="10.5" hidden="1" customHeight="1">
       <c r="A91" s="33">
-        <v>119.0</v>
+        <v>120.0</v>
       </c>
       <c r="B91" s="33" t="s">
         <v>46</v>
@@ -8661,7 +8682,7 @@
     </row>
     <row r="92" ht="10.5" hidden="1" customHeight="1">
       <c r="A92" s="33">
-        <v>120.0</v>
+        <v>121.0</v>
       </c>
       <c r="B92" s="33" t="s">
         <v>46</v>
@@ -8698,13 +8719,13 @@
     </row>
     <row r="93" ht="10.5" hidden="1" customHeight="1">
       <c r="A93" s="33">
-        <v>121.0</v>
+        <v>123.0</v>
       </c>
       <c r="B93" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C93" s="40" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D93" s="33" t="s">
         <v>217</v>
@@ -8735,7 +8756,7 @@
     </row>
     <row r="94" ht="10.5" hidden="1" customHeight="1">
       <c r="A94" s="33">
-        <v>123.0</v>
+        <v>125.0</v>
       </c>
       <c r="B94" s="33" t="s">
         <v>46</v>
@@ -8772,7 +8793,7 @@
     </row>
     <row r="95" ht="10.5" hidden="1" customHeight="1">
       <c r="A95" s="33">
-        <v>125.0</v>
+        <v>126.0</v>
       </c>
       <c r="B95" s="33" t="s">
         <v>46</v>
@@ -8809,7 +8830,7 @@
     </row>
     <row r="96" ht="10.5" hidden="1" customHeight="1">
       <c r="A96" s="33">
-        <v>126.0</v>
+        <v>127.0</v>
       </c>
       <c r="B96" s="33" t="s">
         <v>46</v>
@@ -8846,7 +8867,7 @@
     </row>
     <row r="97" ht="10.5" hidden="1" customHeight="1">
       <c r="A97" s="33">
-        <v>127.0</v>
+        <v>128.0</v>
       </c>
       <c r="B97" s="33" t="s">
         <v>46</v>
@@ -8883,7 +8904,7 @@
     </row>
     <row r="98" ht="10.5" hidden="1" customHeight="1">
       <c r="A98" s="33">
-        <v>128.0</v>
+        <v>129.0</v>
       </c>
       <c r="B98" s="33" t="s">
         <v>46</v>
@@ -8920,7 +8941,7 @@
     </row>
     <row r="99" ht="10.5" hidden="1" customHeight="1">
       <c r="A99" s="33">
-        <v>129.0</v>
+        <v>130.0</v>
       </c>
       <c r="B99" s="33" t="s">
         <v>46</v>
@@ -8957,7 +8978,7 @@
     </row>
     <row r="100" ht="10.5" hidden="1" customHeight="1">
       <c r="A100" s="33">
-        <v>130.0</v>
+        <v>131.0</v>
       </c>
       <c r="B100" s="33" t="s">
         <v>46</v>
@@ -8994,7 +9015,7 @@
     </row>
     <row r="101" ht="10.5" hidden="1" customHeight="1">
       <c r="A101" s="33">
-        <v>131.0</v>
+        <v>132.0</v>
       </c>
       <c r="B101" s="33" t="s">
         <v>46</v>
@@ -9031,7 +9052,7 @@
     </row>
     <row r="102" ht="10.5" hidden="1" customHeight="1">
       <c r="A102" s="33">
-        <v>132.0</v>
+        <v>133.0</v>
       </c>
       <c r="B102" s="33" t="s">
         <v>46</v>
@@ -9068,7 +9089,7 @@
     </row>
     <row r="103" ht="10.5" hidden="1" customHeight="1">
       <c r="A103" s="33">
-        <v>133.0</v>
+        <v>134.0</v>
       </c>
       <c r="B103" s="33" t="s">
         <v>46</v>
@@ -9105,7 +9126,7 @@
     </row>
     <row r="104" ht="10.5" hidden="1" customHeight="1">
       <c r="A104" s="33">
-        <v>134.0</v>
+        <v>135.0</v>
       </c>
       <c r="B104" s="33" t="s">
         <v>46</v>
@@ -9142,7 +9163,7 @@
     </row>
     <row r="105" ht="10.5" hidden="1" customHeight="1">
       <c r="A105" s="33">
-        <v>135.0</v>
+        <v>136.0</v>
       </c>
       <c r="B105" s="33" t="s">
         <v>46</v>
@@ -9179,7 +9200,7 @@
     </row>
     <row r="106" ht="10.5" hidden="1" customHeight="1">
       <c r="A106" s="33">
-        <v>136.0</v>
+        <v>137.0</v>
       </c>
       <c r="B106" s="33" t="s">
         <v>46</v>
@@ -9216,7 +9237,7 @@
     </row>
     <row r="107" ht="10.5" hidden="1" customHeight="1">
       <c r="A107" s="33">
-        <v>137.0</v>
+        <v>138.0</v>
       </c>
       <c r="B107" s="33" t="s">
         <v>46</v>
@@ -9253,7 +9274,7 @@
     </row>
     <row r="108" ht="10.5" hidden="1" customHeight="1">
       <c r="A108" s="33">
-        <v>138.0</v>
+        <v>139.0</v>
       </c>
       <c r="B108" s="33" t="s">
         <v>46</v>
@@ -9290,7 +9311,7 @@
     </row>
     <row r="109" ht="10.5" hidden="1" customHeight="1">
       <c r="A109" s="33">
-        <v>139.0</v>
+        <v>140.0</v>
       </c>
       <c r="B109" s="33" t="s">
         <v>46</v>
@@ -9327,7 +9348,7 @@
     </row>
     <row r="110" ht="10.5" hidden="1" customHeight="1">
       <c r="A110" s="33">
-        <v>140.0</v>
+        <v>141.0</v>
       </c>
       <c r="B110" s="33" t="s">
         <v>46</v>
@@ -9364,7 +9385,7 @@
     </row>
     <row r="111" ht="10.5" hidden="1" customHeight="1">
       <c r="A111" s="33">
-        <v>141.0</v>
+        <v>142.0</v>
       </c>
       <c r="B111" s="33" t="s">
         <v>46</v>
@@ -9401,7 +9422,7 @@
     </row>
     <row r="112" ht="10.5" hidden="1" customHeight="1">
       <c r="A112" s="33">
-        <v>142.0</v>
+        <v>143.0</v>
       </c>
       <c r="B112" s="33" t="s">
         <v>46</v>
@@ -9438,7 +9459,7 @@
     </row>
     <row r="113" ht="10.5" hidden="1" customHeight="1">
       <c r="A113" s="33">
-        <v>143.0</v>
+        <v>144.0</v>
       </c>
       <c r="B113" s="33" t="s">
         <v>46</v>
@@ -9475,7 +9496,7 @@
     </row>
     <row r="114" ht="10.5" hidden="1" customHeight="1">
       <c r="A114" s="33">
-        <v>144.0</v>
+        <v>145.0</v>
       </c>
       <c r="B114" s="33" t="s">
         <v>46</v>
@@ -9512,7 +9533,7 @@
     </row>
     <row r="115" ht="10.5" hidden="1" customHeight="1">
       <c r="A115" s="33">
-        <v>145.0</v>
+        <v>146.0</v>
       </c>
       <c r="B115" s="33" t="s">
         <v>46</v>
@@ -9549,13 +9570,13 @@
     </row>
     <row r="116" ht="10.5" hidden="1" customHeight="1">
       <c r="A116" s="33">
-        <v>146.0</v>
+        <v>152.0</v>
       </c>
       <c r="B116" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C116" s="40" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D116" s="33" t="s">
         <v>263</v>
@@ -9586,7 +9607,7 @@
     </row>
     <row r="117" ht="10.5" hidden="1" customHeight="1">
       <c r="A117" s="33">
-        <v>152.0</v>
+        <v>154.0</v>
       </c>
       <c r="B117" s="33" t="s">
         <v>46</v>
@@ -9623,7 +9644,7 @@
     </row>
     <row r="118" ht="10.5" hidden="1" customHeight="1">
       <c r="A118" s="33">
-        <v>154.0</v>
+        <v>155.0</v>
       </c>
       <c r="B118" s="33" t="s">
         <v>46</v>
@@ -9660,7 +9681,7 @@
     </row>
     <row r="119" ht="10.5" hidden="1" customHeight="1">
       <c r="A119" s="33">
-        <v>155.0</v>
+        <v>156.0</v>
       </c>
       <c r="B119" s="33" t="s">
         <v>46</v>
@@ -9697,7 +9718,7 @@
     </row>
     <row r="120" ht="10.5" hidden="1" customHeight="1">
       <c r="A120" s="33">
-        <v>156.0</v>
+        <v>159.0</v>
       </c>
       <c r="B120" s="33" t="s">
         <v>46</v>
@@ -9734,7 +9755,7 @@
     </row>
     <row r="121" ht="10.5" hidden="1" customHeight="1">
       <c r="A121" s="33">
-        <v>158.0</v>
+        <v>160.0</v>
       </c>
       <c r="B121" s="33" t="s">
         <v>46</v>
@@ -9771,7 +9792,7 @@
     </row>
     <row r="122" ht="10.5" hidden="1" customHeight="1">
       <c r="A122" s="33">
-        <v>159.0</v>
+        <v>161.0</v>
       </c>
       <c r="B122" s="33" t="s">
         <v>46</v>
@@ -9808,7 +9829,7 @@
     </row>
     <row r="123" ht="10.5" hidden="1" customHeight="1">
       <c r="A123" s="33">
-        <v>160.0</v>
+        <v>162.0</v>
       </c>
       <c r="B123" s="33" t="s">
         <v>46</v>
@@ -9845,7 +9866,7 @@
     </row>
     <row r="124" ht="10.5" hidden="1" customHeight="1">
       <c r="A124" s="33">
-        <v>161.0</v>
+        <v>163.0</v>
       </c>
       <c r="B124" s="33" t="s">
         <v>46</v>
@@ -9882,7 +9903,7 @@
     </row>
     <row r="125" ht="10.5" hidden="1" customHeight="1">
       <c r="A125" s="33">
-        <v>162.0</v>
+        <v>164.0</v>
       </c>
       <c r="B125" s="33" t="s">
         <v>46</v>
@@ -9919,7 +9940,7 @@
     </row>
     <row r="126" ht="10.5" hidden="1" customHeight="1">
       <c r="A126" s="33">
-        <v>163.0</v>
+        <v>165.0</v>
       </c>
       <c r="B126" s="33" t="s">
         <v>46</v>
@@ -9956,7 +9977,7 @@
     </row>
     <row r="127" ht="10.5" hidden="1" customHeight="1">
       <c r="A127" s="33">
-        <v>164.0</v>
+        <v>166.0</v>
       </c>
       <c r="B127" s="33" t="s">
         <v>46</v>
@@ -9993,7 +10014,7 @@
     </row>
     <row r="128" ht="10.5" hidden="1" customHeight="1">
       <c r="A128" s="33">
-        <v>165.0</v>
+        <v>167.0</v>
       </c>
       <c r="B128" s="33" t="s">
         <v>46</v>
@@ -10030,7 +10051,7 @@
     </row>
     <row r="129" ht="10.5" hidden="1" customHeight="1">
       <c r="A129" s="33">
-        <v>166.0</v>
+        <v>168.0</v>
       </c>
       <c r="B129" s="33" t="s">
         <v>46</v>
@@ -10067,7 +10088,7 @@
     </row>
     <row r="130" ht="10.5" hidden="1" customHeight="1">
       <c r="A130" s="33">
-        <v>167.0</v>
+        <v>169.0</v>
       </c>
       <c r="B130" s="33" t="s">
         <v>46</v>
@@ -10104,13 +10125,13 @@
     </row>
     <row r="131" ht="10.5" hidden="1" customHeight="1">
       <c r="A131" s="33">
-        <v>168.0</v>
+        <v>175.0</v>
       </c>
       <c r="B131" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C131" s="40" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D131" s="33" t="s">
         <v>293</v>
@@ -10141,13 +10162,13 @@
     </row>
     <row r="132" ht="10.5" hidden="1" customHeight="1">
       <c r="A132" s="33">
-        <v>169.0</v>
+        <v>177.0</v>
       </c>
       <c r="B132" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C132" s="40" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D132" s="33" t="s">
         <v>295</v>
@@ -10178,7 +10199,7 @@
     </row>
     <row r="133" ht="10.5" hidden="1" customHeight="1">
       <c r="A133" s="33">
-        <v>175.0</v>
+        <v>178.0</v>
       </c>
       <c r="B133" s="33" t="s">
         <v>46</v>
@@ -10215,7 +10236,7 @@
     </row>
     <row r="134" ht="10.5" hidden="1" customHeight="1">
       <c r="A134" s="33">
-        <v>177.0</v>
+        <v>179.0</v>
       </c>
       <c r="B134" s="33" t="s">
         <v>46</v>
@@ -10252,7 +10273,7 @@
     </row>
     <row r="135" ht="10.5" hidden="1" customHeight="1">
       <c r="A135" s="33">
-        <v>178.0</v>
+        <v>180.0</v>
       </c>
       <c r="B135" s="33" t="s">
         <v>46</v>
@@ -10289,7 +10310,7 @@
     </row>
     <row r="136" ht="10.5" hidden="1" customHeight="1">
       <c r="A136" s="33">
-        <v>179.0</v>
+        <v>181.0</v>
       </c>
       <c r="B136" s="33" t="s">
         <v>46</v>
@@ -10326,7 +10347,7 @@
     </row>
     <row r="137" ht="10.5" hidden="1" customHeight="1">
       <c r="A137" s="33">
-        <v>180.0</v>
+        <v>182.0</v>
       </c>
       <c r="B137" s="33" t="s">
         <v>46</v>
@@ -10363,7 +10384,7 @@
     </row>
     <row r="138" ht="10.5" hidden="1" customHeight="1">
       <c r="A138" s="33">
-        <v>181.0</v>
+        <v>183.0</v>
       </c>
       <c r="B138" s="33" t="s">
         <v>46</v>
@@ -10400,7 +10421,7 @@
     </row>
     <row r="139" ht="10.5" hidden="1" customHeight="1">
       <c r="A139" s="33">
-        <v>182.0</v>
+        <v>184.0</v>
       </c>
       <c r="B139" s="33" t="s">
         <v>46</v>
@@ -10437,7 +10458,7 @@
     </row>
     <row r="140" ht="10.5" hidden="1" customHeight="1">
       <c r="A140" s="33">
-        <v>183.0</v>
+        <v>185.0</v>
       </c>
       <c r="B140" s="33" t="s">
         <v>46</v>
@@ -10474,7 +10495,7 @@
     </row>
     <row r="141" ht="10.5" hidden="1" customHeight="1">
       <c r="A141" s="33">
-        <v>184.0</v>
+        <v>186.0</v>
       </c>
       <c r="B141" s="33" t="s">
         <v>46</v>
@@ -10511,7 +10532,7 @@
     </row>
     <row r="142" ht="10.5" hidden="1" customHeight="1">
       <c r="A142" s="33">
-        <v>185.0</v>
+        <v>187.0</v>
       </c>
       <c r="B142" s="33" t="s">
         <v>46</v>
@@ -10548,7 +10569,7 @@
     </row>
     <row r="143" ht="10.5" hidden="1" customHeight="1">
       <c r="A143" s="33">
-        <v>186.0</v>
+        <v>188.0</v>
       </c>
       <c r="B143" s="33" t="s">
         <v>46</v>
@@ -10585,7 +10606,7 @@
     </row>
     <row r="144" ht="10.5" hidden="1" customHeight="1">
       <c r="A144" s="33">
-        <v>187.0</v>
+        <v>189.0</v>
       </c>
       <c r="B144" s="33" t="s">
         <v>46</v>
@@ -10622,7 +10643,7 @@
     </row>
     <row r="145" ht="10.5" hidden="1" customHeight="1">
       <c r="A145" s="33">
-        <v>188.0</v>
+        <v>190.0</v>
       </c>
       <c r="B145" s="33" t="s">
         <v>46</v>
@@ -10659,13 +10680,13 @@
     </row>
     <row r="146" ht="10.5" hidden="1" customHeight="1">
       <c r="A146" s="33">
-        <v>189.0</v>
+        <v>191.0</v>
       </c>
       <c r="B146" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C146" s="40" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D146" s="33" t="s">
         <v>323</v>
@@ -10691,18 +10712,18 @@
       <c r="U146" s="38"/>
       <c r="V146" s="39"/>
       <c r="W146" s="37" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="147" ht="10.5" hidden="1" customHeight="1">
       <c r="A147" s="33">
-        <v>190.0</v>
+        <v>376.0</v>
       </c>
       <c r="B147" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C147" s="40" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D147" s="33" t="s">
         <v>325</v>
@@ -10728,739 +10749,791 @@
       <c r="U147" s="38"/>
       <c r="V147" s="39"/>
       <c r="W147" s="37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="148" ht="10.5" customHeight="1">
+      <c r="A148" s="42">
+        <v>417.0</v>
+      </c>
+      <c r="B148" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C148" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D148" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E148" s="39" t="s">
+        <v>329</v>
+      </c>
+      <c r="F148" s="44">
+        <v>45805.0</v>
+      </c>
+      <c r="G148" s="44">
+        <v>1.748417867E12</v>
+      </c>
+      <c r="H148" s="44" t="s">
+        <v>330</v>
+      </c>
+      <c r="I148" s="45" t="s">
+        <v>331</v>
+      </c>
+      <c r="J148" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="K148" s="47"/>
+      <c r="L148" s="47"/>
+      <c r="M148" s="47"/>
+      <c r="N148" s="47"/>
+      <c r="O148" s="47"/>
+      <c r="P148" s="47"/>
+      <c r="Q148" s="47"/>
+      <c r="R148" s="47"/>
+      <c r="S148" s="47"/>
+      <c r="T148" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="U148" s="48"/>
+      <c r="V148" s="49"/>
+      <c r="W148" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="X148" s="50"/>
+      <c r="Y148" s="50"/>
+      <c r="Z148" s="50"/>
+    </row>
+    <row r="149" ht="10.5" customHeight="1">
+      <c r="A149" s="42">
+        <v>418.0</v>
+      </c>
+      <c r="B149" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C149" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D149" s="42" t="s">
+        <v>333</v>
+      </c>
+      <c r="E149" s="39" t="s">
+        <v>334</v>
+      </c>
+      <c r="F149" s="44">
+        <v>45805.0</v>
+      </c>
+      <c r="G149" s="44">
+        <v>1.748425607E12</v>
+      </c>
+      <c r="H149" s="44" t="s">
+        <v>335</v>
+      </c>
+      <c r="I149" s="45" t="s">
+        <v>336</v>
+      </c>
+      <c r="J149" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="K149" s="47"/>
+      <c r="L149" s="47"/>
+      <c r="M149" s="47"/>
+      <c r="N149" s="47"/>
+      <c r="O149" s="47"/>
+      <c r="P149" s="47"/>
+      <c r="Q149" s="47"/>
+      <c r="R149" s="47"/>
+      <c r="S149" s="47"/>
+      <c r="T149" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="U149" s="48"/>
+      <c r="V149" s="49"/>
+      <c r="W149" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="X149" s="50"/>
+      <c r="Y149" s="50"/>
+      <c r="Z149" s="50"/>
+    </row>
+    <row r="150" ht="10.5" customHeight="1">
+      <c r="A150" s="42">
+        <v>419.0</v>
+      </c>
+      <c r="B150" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C150" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D150" s="42" t="s">
+        <v>337</v>
+      </c>
+      <c r="E150" s="39" t="s">
+        <v>338</v>
+      </c>
+      <c r="F150" s="44">
+        <v>45805.0</v>
+      </c>
+      <c r="G150" s="44">
+        <v>1.748428247E12</v>
+      </c>
+      <c r="H150" s="44" t="s">
+        <v>339</v>
+      </c>
+      <c r="I150" s="45" t="s">
+        <v>340</v>
+      </c>
+      <c r="J150" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="K150" s="47"/>
+      <c r="L150" s="47"/>
+      <c r="M150" s="47"/>
+      <c r="N150" s="47"/>
+      <c r="O150" s="47"/>
+      <c r="P150" s="47"/>
+      <c r="Q150" s="47"/>
+      <c r="R150" s="47"/>
+      <c r="S150" s="47"/>
+      <c r="T150" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="U150" s="48"/>
+      <c r="V150" s="49"/>
+      <c r="W150" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="X150" s="50"/>
+      <c r="Y150" s="50"/>
+      <c r="Z150" s="50"/>
+    </row>
+    <row r="151" ht="10.5" customHeight="1">
+      <c r="A151" s="42">
+        <v>423.0</v>
+      </c>
+      <c r="B151" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C151" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D151" s="42" t="s">
+        <v>341</v>
+      </c>
+      <c r="E151" s="39" t="s">
+        <v>342</v>
+      </c>
+      <c r="F151" s="51"/>
+      <c r="G151" s="51"/>
+      <c r="H151" s="51"/>
+      <c r="I151" s="52"/>
+      <c r="J151" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="K151" s="47"/>
+      <c r="L151" s="47"/>
+      <c r="M151" s="47"/>
+      <c r="N151" s="47"/>
+      <c r="O151" s="47"/>
+      <c r="P151" s="47"/>
+      <c r="Q151" s="47"/>
+      <c r="R151" s="47"/>
+      <c r="S151" s="47"/>
+      <c r="T151" s="47"/>
+      <c r="U151" s="48"/>
+      <c r="V151" s="49"/>
+      <c r="W151" s="46" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="148" ht="10.5" hidden="1" customHeight="1">
-      <c r="A148" s="33">
-        <v>191.0</v>
-      </c>
-      <c r="B148" s="33" t="s">
+      <c r="X151" s="50"/>
+      <c r="Y151" s="50"/>
+      <c r="Z151" s="50"/>
+    </row>
+    <row r="152" ht="10.5" customHeight="1">
+      <c r="A152" s="42">
+        <v>424.0</v>
+      </c>
+      <c r="B152" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C148" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D148" s="33" t="s">
+      <c r="C152" s="43" t="s">
         <v>327</v>
       </c>
-      <c r="E148" s="34" t="s">
-        <v>328</v>
-      </c>
-      <c r="F148" s="36"/>
-      <c r="G148" s="36"/>
-      <c r="H148" s="36"/>
-      <c r="I148" s="41"/>
-      <c r="J148" s="37"/>
-      <c r="K148" s="37"/>
-      <c r="L148" s="37"/>
-      <c r="M148" s="37"/>
-      <c r="N148" s="37"/>
-      <c r="O148" s="37"/>
-      <c r="P148" s="37"/>
-      <c r="Q148" s="37"/>
-      <c r="R148" s="37"/>
-      <c r="S148" s="37"/>
-      <c r="T148" s="37"/>
-      <c r="U148" s="38"/>
-      <c r="V148" s="39"/>
-      <c r="W148" s="37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="149" ht="10.5" hidden="1" customHeight="1">
-      <c r="A149" s="33">
-        <v>376.0</v>
-      </c>
-      <c r="B149" s="33" t="s">
+      <c r="D152" s="42" t="s">
+        <v>344</v>
+      </c>
+      <c r="E152" s="39" t="s">
+        <v>345</v>
+      </c>
+      <c r="F152" s="44">
+        <v>45805.0</v>
+      </c>
+      <c r="G152" s="44">
+        <v>1.748435747E12</v>
+      </c>
+      <c r="H152" s="44" t="s">
+        <v>346</v>
+      </c>
+      <c r="I152" s="45" t="s">
+        <v>347</v>
+      </c>
+      <c r="J152" s="47"/>
+      <c r="K152" s="47"/>
+      <c r="L152" s="47"/>
+      <c r="M152" s="47"/>
+      <c r="N152" s="47"/>
+      <c r="O152" s="46" t="s">
+        <v>348</v>
+      </c>
+      <c r="P152" s="47"/>
+      <c r="Q152" s="47"/>
+      <c r="R152" s="47"/>
+      <c r="S152" s="47"/>
+      <c r="T152" s="46" t="s">
+        <v>349</v>
+      </c>
+      <c r="U152" s="48"/>
+      <c r="V152" s="49"/>
+      <c r="W152" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="X152" s="50"/>
+      <c r="Y152" s="50"/>
+      <c r="Z152" s="50"/>
+    </row>
+    <row r="153" ht="10.5" customHeight="1">
+      <c r="A153" s="42">
+        <v>425.0</v>
+      </c>
+      <c r="B153" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C149" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D149" s="33" t="s">
-        <v>329</v>
-      </c>
-      <c r="E149" s="34" t="s">
-        <v>330</v>
-      </c>
-      <c r="F149" s="36"/>
-      <c r="G149" s="36"/>
-      <c r="H149" s="36"/>
-      <c r="I149" s="41"/>
-      <c r="J149" s="37"/>
-      <c r="K149" s="37"/>
-      <c r="L149" s="37"/>
-      <c r="M149" s="37"/>
-      <c r="N149" s="37"/>
-      <c r="O149" s="37"/>
-      <c r="P149" s="37"/>
-      <c r="Q149" s="37"/>
-      <c r="R149" s="37"/>
-      <c r="S149" s="37"/>
-      <c r="T149" s="37"/>
-      <c r="U149" s="38"/>
-      <c r="V149" s="39"/>
-      <c r="W149" s="37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="150" ht="10.5" hidden="1" customHeight="1">
-      <c r="A150" s="33">
-        <v>417.0</v>
-      </c>
-      <c r="B150" s="33" t="s">
+      <c r="C153" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D153" s="42" t="s">
+        <v>350</v>
+      </c>
+      <c r="E153" s="39" t="s">
+        <v>351</v>
+      </c>
+      <c r="F153" s="51"/>
+      <c r="G153" s="51"/>
+      <c r="H153" s="51"/>
+      <c r="I153" s="52"/>
+      <c r="J153" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="K153" s="47"/>
+      <c r="L153" s="47"/>
+      <c r="M153" s="47"/>
+      <c r="N153" s="47"/>
+      <c r="O153" s="47"/>
+      <c r="P153" s="47"/>
+      <c r="Q153" s="47"/>
+      <c r="R153" s="47"/>
+      <c r="S153" s="47"/>
+      <c r="T153" s="47"/>
+      <c r="U153" s="48"/>
+      <c r="V153" s="49"/>
+      <c r="W153" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="X153" s="50"/>
+      <c r="Y153" s="50"/>
+      <c r="Z153" s="50"/>
+    </row>
+    <row r="154" ht="10.5" customHeight="1">
+      <c r="A154" s="42">
+        <v>432.0</v>
+      </c>
+      <c r="B154" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C150" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D150" s="33" t="s">
-        <v>332</v>
-      </c>
-      <c r="E150" s="34" t="s">
-        <v>333</v>
-      </c>
-      <c r="F150" s="36">
+      <c r="C154" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D154" s="42" t="s">
+        <v>352</v>
+      </c>
+      <c r="E154" s="39" t="s">
+        <v>353</v>
+      </c>
+      <c r="F154" s="44">
         <v>45805.0</v>
       </c>
-      <c r="G150" s="42">
-        <v>1.748417867E12</v>
-      </c>
-      <c r="H150" s="42" t="s">
-        <v>334</v>
-      </c>
-      <c r="I150" s="43" t="s">
-        <v>335</v>
-      </c>
-      <c r="J150" s="44" t="s">
+      <c r="G154" s="44">
+        <v>1.748434847E12</v>
+      </c>
+      <c r="H154" s="44" t="s">
+        <v>354</v>
+      </c>
+      <c r="I154" s="45" t="s">
+        <v>355</v>
+      </c>
+      <c r="J154" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="K150" s="37"/>
-      <c r="L150" s="37"/>
-      <c r="M150" s="37"/>
-      <c r="N150" s="37"/>
-      <c r="O150" s="37"/>
-      <c r="P150" s="37"/>
-      <c r="Q150" s="37"/>
-      <c r="R150" s="37"/>
-      <c r="S150" s="37"/>
-      <c r="T150" s="44" t="s">
-        <v>336</v>
-      </c>
-      <c r="U150" s="38"/>
-      <c r="V150" s="39"/>
-      <c r="W150" s="37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="151" ht="10.5" hidden="1" customHeight="1">
-      <c r="A151" s="33">
-        <v>418.0</v>
-      </c>
-      <c r="B151" s="33" t="s">
+      <c r="K154" s="47"/>
+      <c r="L154" s="47"/>
+      <c r="M154" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="N154" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="O154" s="46" t="s">
+        <v>356</v>
+      </c>
+      <c r="P154" s="47"/>
+      <c r="Q154" s="47"/>
+      <c r="R154" s="47"/>
+      <c r="S154" s="47"/>
+      <c r="T154" s="46" t="s">
+        <v>349</v>
+      </c>
+      <c r="U154" s="48"/>
+      <c r="V154" s="49"/>
+      <c r="W154" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="X154" s="50"/>
+      <c r="Y154" s="50"/>
+      <c r="Z154" s="50"/>
+    </row>
+    <row r="155" ht="10.5" customHeight="1">
+      <c r="A155" s="42">
+        <v>433.0</v>
+      </c>
+      <c r="B155" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C151" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D151" s="33" t="s">
-        <v>337</v>
-      </c>
-      <c r="E151" s="34" t="s">
-        <v>338</v>
-      </c>
-      <c r="F151" s="36">
+      <c r="C155" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D155" s="42" t="s">
+        <v>357</v>
+      </c>
+      <c r="E155" s="39" t="s">
+        <v>358</v>
+      </c>
+      <c r="F155" s="51"/>
+      <c r="G155" s="51"/>
+      <c r="H155" s="51"/>
+      <c r="I155" s="52"/>
+      <c r="J155" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="K155" s="46" t="s">
+        <v>359</v>
+      </c>
+      <c r="L155" s="47"/>
+      <c r="M155" s="47"/>
+      <c r="N155" s="47"/>
+      <c r="O155" s="47"/>
+      <c r="P155" s="47"/>
+      <c r="Q155" s="47"/>
+      <c r="R155" s="47"/>
+      <c r="S155" s="47"/>
+      <c r="T155" s="47"/>
+      <c r="U155" s="48"/>
+      <c r="V155" s="49"/>
+      <c r="W155" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="X155" s="50"/>
+      <c r="Y155" s="50"/>
+      <c r="Z155" s="50"/>
+    </row>
+    <row r="156" ht="10.5" customHeight="1">
+      <c r="A156" s="42">
+        <v>434.0</v>
+      </c>
+      <c r="B156" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C156" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D156" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="E156" s="39" t="s">
+        <v>361</v>
+      </c>
+      <c r="F156" s="51"/>
+      <c r="G156" s="51"/>
+      <c r="H156" s="51"/>
+      <c r="I156" s="52"/>
+      <c r="J156" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="K156" s="46" t="s">
+        <v>359</v>
+      </c>
+      <c r="L156" s="47"/>
+      <c r="M156" s="47"/>
+      <c r="N156" s="47"/>
+      <c r="O156" s="47"/>
+      <c r="P156" s="47"/>
+      <c r="Q156" s="47"/>
+      <c r="R156" s="47"/>
+      <c r="S156" s="47"/>
+      <c r="T156" s="46" t="s">
+        <v>349</v>
+      </c>
+      <c r="U156" s="48"/>
+      <c r="V156" s="49"/>
+      <c r="W156" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="X156" s="50"/>
+      <c r="Y156" s="50"/>
+      <c r="Z156" s="50"/>
+    </row>
+    <row r="157" ht="10.5" customHeight="1">
+      <c r="A157" s="42">
+        <v>435.0</v>
+      </c>
+      <c r="B157" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C157" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D157" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="E157" s="39" t="s">
+        <v>363</v>
+      </c>
+      <c r="F157" s="44">
         <v>45805.0</v>
       </c>
-      <c r="G151" s="42">
-        <v>1.748425607E12</v>
-      </c>
-      <c r="H151" s="42" t="s">
-        <v>339</v>
-      </c>
-      <c r="I151" s="43" t="s">
-        <v>340</v>
-      </c>
-      <c r="J151" s="44" t="s">
+      <c r="G157" s="44">
+        <v>1.748438752E12</v>
+      </c>
+      <c r="H157" s="44" t="s">
+        <v>364</v>
+      </c>
+      <c r="I157" s="45" t="s">
+        <v>365</v>
+      </c>
+      <c r="J157" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="K151" s="37"/>
-      <c r="L151" s="37"/>
-      <c r="M151" s="37"/>
-      <c r="N151" s="37"/>
-      <c r="O151" s="37"/>
-      <c r="P151" s="37"/>
-      <c r="Q151" s="37"/>
-      <c r="R151" s="37"/>
-      <c r="S151" s="37"/>
-      <c r="T151" s="44" t="s">
-        <v>336</v>
-      </c>
-      <c r="U151" s="38"/>
-      <c r="V151" s="39"/>
-      <c r="W151" s="37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="152" ht="10.5" hidden="1" customHeight="1">
-      <c r="A152" s="33">
-        <v>419.0</v>
-      </c>
-      <c r="B152" s="33" t="s">
+      <c r="K157" s="47"/>
+      <c r="L157" s="47"/>
+      <c r="M157" s="47"/>
+      <c r="N157" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="O157" s="46" t="s">
+        <v>366</v>
+      </c>
+      <c r="P157" s="47"/>
+      <c r="Q157" s="47"/>
+      <c r="R157" s="47"/>
+      <c r="S157" s="47"/>
+      <c r="T157" s="46" t="s">
+        <v>349</v>
+      </c>
+      <c r="U157" s="48"/>
+      <c r="V157" s="49"/>
+      <c r="W157" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="X157" s="50"/>
+      <c r="Y157" s="50"/>
+      <c r="Z157" s="50"/>
+    </row>
+    <row r="158" ht="10.5" customHeight="1">
+      <c r="A158" s="42">
+        <v>437.0</v>
+      </c>
+      <c r="B158" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C152" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D152" s="33" t="s">
-        <v>341</v>
-      </c>
-      <c r="E152" s="34" t="s">
-        <v>342</v>
-      </c>
-      <c r="F152" s="36">
-        <v>45805.0</v>
-      </c>
-      <c r="G152" s="42">
-        <v>1.748428247E12</v>
-      </c>
-      <c r="H152" s="42" t="s">
+      <c r="C158" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D158" s="42" t="s">
+        <v>367</v>
+      </c>
+      <c r="E158" s="39" t="s">
+        <v>368</v>
+      </c>
+      <c r="F158" s="53"/>
+      <c r="G158" s="51"/>
+      <c r="H158" s="51"/>
+      <c r="I158" s="52"/>
+      <c r="J158" s="46" t="s">
         <v>343</v>
       </c>
-      <c r="I152" s="43" t="s">
-        <v>344</v>
-      </c>
-      <c r="J152" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="K152" s="37"/>
-      <c r="L152" s="37"/>
-      <c r="M152" s="37"/>
-      <c r="N152" s="37"/>
-      <c r="O152" s="37"/>
-      <c r="P152" s="37"/>
-      <c r="Q152" s="37"/>
-      <c r="R152" s="37"/>
-      <c r="S152" s="37"/>
-      <c r="T152" s="44" t="s">
-        <v>336</v>
-      </c>
-      <c r="U152" s="38"/>
-      <c r="V152" s="39"/>
-      <c r="W152" s="37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="153" ht="10.5" customHeight="1">
-      <c r="A153" s="33">
-        <v>423.0</v>
-      </c>
-      <c r="B153" s="33" t="s">
+      <c r="K158" s="46" t="s">
+        <v>369</v>
+      </c>
+      <c r="L158" s="47"/>
+      <c r="M158" s="47"/>
+      <c r="N158" s="47"/>
+      <c r="O158" s="47"/>
+      <c r="P158" s="47"/>
+      <c r="Q158" s="47"/>
+      <c r="R158" s="47"/>
+      <c r="S158" s="47"/>
+      <c r="T158" s="47"/>
+      <c r="U158" s="48"/>
+      <c r="V158" s="49"/>
+      <c r="W158" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="X158" s="50"/>
+      <c r="Y158" s="50"/>
+      <c r="Z158" s="50"/>
+    </row>
+    <row r="159" ht="10.5" customHeight="1">
+      <c r="A159" s="42">
+        <v>438.0</v>
+      </c>
+      <c r="B159" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C153" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D153" s="33" t="s">
-        <v>345</v>
-      </c>
-      <c r="E153" s="34" t="s">
-        <v>346</v>
-      </c>
-      <c r="F153" s="36"/>
-      <c r="G153" s="36"/>
-      <c r="H153" s="36"/>
-      <c r="I153" s="41"/>
-      <c r="J153" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="K153" s="37"/>
-      <c r="L153" s="37"/>
-      <c r="M153" s="37"/>
-      <c r="N153" s="37"/>
-      <c r="O153" s="37"/>
-      <c r="P153" s="37"/>
-      <c r="Q153" s="37"/>
-      <c r="R153" s="37"/>
-      <c r="S153" s="37"/>
-      <c r="T153" s="37"/>
-      <c r="U153" s="38"/>
-      <c r="V153" s="39"/>
-      <c r="W153" s="37" t="s">
+      <c r="C159" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D159" s="42" t="s">
+        <v>370</v>
+      </c>
+      <c r="E159" s="39" t="s">
+        <v>371</v>
+      </c>
+      <c r="F159" s="51"/>
+      <c r="G159" s="51"/>
+      <c r="H159" s="51"/>
+      <c r="I159" s="52"/>
+      <c r="J159" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="K159" s="46" t="s">
+        <v>369</v>
+      </c>
+      <c r="L159" s="47"/>
+      <c r="M159" s="47"/>
+      <c r="N159" s="47"/>
+      <c r="O159" s="47"/>
+      <c r="P159" s="47"/>
+      <c r="Q159" s="47"/>
+      <c r="R159" s="47"/>
+      <c r="S159" s="47"/>
+      <c r="T159" s="47"/>
+      <c r="U159" s="48"/>
+      <c r="V159" s="49"/>
+      <c r="W159" s="46" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="154" ht="10.5" customHeight="1">
-      <c r="A154" s="33">
-        <v>424.0</v>
-      </c>
-      <c r="B154" s="33" t="s">
+      <c r="X159" s="50"/>
+      <c r="Y159" s="50"/>
+      <c r="Z159" s="50"/>
+    </row>
+    <row r="160" ht="10.5" customHeight="1">
+      <c r="A160" s="42">
+        <v>440.0</v>
+      </c>
+      <c r="B160" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C154" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D154" s="33" t="s">
-        <v>348</v>
-      </c>
-      <c r="E154" s="34" t="s">
-        <v>349</v>
-      </c>
-      <c r="F154" s="36">
-        <v>45805.0</v>
-      </c>
-      <c r="G154" s="42">
-        <v>1.748435747E12</v>
-      </c>
-      <c r="H154" s="42" t="s">
-        <v>350</v>
-      </c>
-      <c r="I154" s="43" t="s">
-        <v>351</v>
-      </c>
-      <c r="J154" s="37"/>
-      <c r="K154" s="37"/>
-      <c r="L154" s="37"/>
-      <c r="M154" s="37"/>
-      <c r="N154" s="37"/>
-      <c r="O154" s="44" t="s">
-        <v>352</v>
-      </c>
-      <c r="P154" s="37"/>
-      <c r="Q154" s="37"/>
-      <c r="R154" s="37"/>
-      <c r="S154" s="37"/>
-      <c r="T154" s="44" t="s">
-        <v>353</v>
-      </c>
-      <c r="U154" s="38"/>
-      <c r="V154" s="39"/>
-      <c r="W154" s="37" t="s">
+      <c r="C160" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D160" s="42" t="s">
+        <v>372</v>
+      </c>
+      <c r="E160" s="39" t="s">
+        <v>373</v>
+      </c>
+      <c r="F160" s="51"/>
+      <c r="G160" s="51"/>
+      <c r="H160" s="51"/>
+      <c r="I160" s="52"/>
+      <c r="J160" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="K160" s="46" t="s">
+        <v>369</v>
+      </c>
+      <c r="L160" s="47"/>
+      <c r="M160" s="47"/>
+      <c r="N160" s="47"/>
+      <c r="O160" s="47"/>
+      <c r="P160" s="47"/>
+      <c r="Q160" s="47"/>
+      <c r="R160" s="47"/>
+      <c r="S160" s="47"/>
+      <c r="T160" s="47"/>
+      <c r="U160" s="48"/>
+      <c r="V160" s="49"/>
+      <c r="W160" s="46" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="155" ht="10.5" customHeight="1">
-      <c r="A155" s="33">
-        <v>425.0</v>
-      </c>
-      <c r="B155" s="33" t="s">
+      <c r="X160" s="50"/>
+      <c r="Y160" s="50"/>
+      <c r="Z160" s="50"/>
+    </row>
+    <row r="161" ht="10.5" customHeight="1">
+      <c r="A161" s="42">
+        <v>441.0</v>
+      </c>
+      <c r="B161" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C155" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D155" s="33" t="s">
-        <v>354</v>
-      </c>
-      <c r="E155" s="34" t="s">
-        <v>355</v>
-      </c>
-      <c r="F155" s="36"/>
-      <c r="G155" s="36"/>
-      <c r="H155" s="36"/>
-      <c r="I155" s="41"/>
-      <c r="J155" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="K155" s="37"/>
-      <c r="L155" s="37"/>
-      <c r="M155" s="37"/>
-      <c r="N155" s="37"/>
-      <c r="O155" s="37"/>
-      <c r="P155" s="37"/>
-      <c r="Q155" s="37"/>
-      <c r="R155" s="37"/>
-      <c r="S155" s="37"/>
-      <c r="T155" s="37"/>
-      <c r="U155" s="38"/>
-      <c r="V155" s="39"/>
-      <c r="W155" s="37" t="s">
+      <c r="C161" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D161" s="42" t="s">
+        <v>374</v>
+      </c>
+      <c r="E161" s="39" t="s">
+        <v>375</v>
+      </c>
+      <c r="F161" s="51"/>
+      <c r="G161" s="51"/>
+      <c r="H161" s="51"/>
+      <c r="I161" s="52"/>
+      <c r="J161" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="K161" s="46" t="s">
+        <v>369</v>
+      </c>
+      <c r="L161" s="47"/>
+      <c r="M161" s="47"/>
+      <c r="N161" s="47"/>
+      <c r="O161" s="47"/>
+      <c r="P161" s="47"/>
+      <c r="Q161" s="47"/>
+      <c r="R161" s="47"/>
+      <c r="S161" s="47"/>
+      <c r="T161" s="47"/>
+      <c r="U161" s="48"/>
+      <c r="V161" s="49"/>
+      <c r="W161" s="46" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="156" ht="10.5" customHeight="1">
-      <c r="A156" s="33">
-        <v>432.0</v>
-      </c>
-      <c r="B156" s="33" t="s">
+      <c r="X161" s="50"/>
+      <c r="Y161" s="50"/>
+      <c r="Z161" s="50"/>
+    </row>
+    <row r="162" ht="10.5" customHeight="1">
+      <c r="A162" s="42">
+        <v>442.0</v>
+      </c>
+      <c r="B162" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C156" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D156" s="33" t="s">
-        <v>356</v>
-      </c>
-      <c r="E156" s="34" t="s">
-        <v>357</v>
-      </c>
-      <c r="F156" s="36">
-        <v>45805.0</v>
-      </c>
-      <c r="G156" s="42">
-        <v>1.748434847E12</v>
-      </c>
-      <c r="H156" s="42" t="s">
-        <v>358</v>
-      </c>
-      <c r="I156" s="43" t="s">
-        <v>359</v>
-      </c>
-      <c r="J156" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="K156" s="37"/>
-      <c r="L156" s="37"/>
-      <c r="M156" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="N156" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="O156" s="44" t="s">
-        <v>360</v>
-      </c>
-      <c r="P156" s="37"/>
-      <c r="Q156" s="37"/>
-      <c r="R156" s="37"/>
-      <c r="S156" s="37"/>
-      <c r="T156" s="44" t="s">
-        <v>353</v>
-      </c>
-      <c r="U156" s="38"/>
-      <c r="V156" s="39"/>
-      <c r="W156" s="37" t="s">
+      <c r="C162" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D162" s="42" t="s">
+        <v>376</v>
+      </c>
+      <c r="E162" s="39" t="s">
+        <v>377</v>
+      </c>
+      <c r="F162" s="51"/>
+      <c r="G162" s="51"/>
+      <c r="H162" s="51"/>
+      <c r="I162" s="52"/>
+      <c r="J162" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="K162" s="46" t="s">
+        <v>378</v>
+      </c>
+      <c r="L162" s="47"/>
+      <c r="M162" s="47"/>
+      <c r="N162" s="47"/>
+      <c r="O162" s="47"/>
+      <c r="P162" s="47"/>
+      <c r="Q162" s="47"/>
+      <c r="R162" s="47"/>
+      <c r="S162" s="47"/>
+      <c r="T162" s="47"/>
+      <c r="U162" s="48"/>
+      <c r="V162" s="49"/>
+      <c r="W162" s="46" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="157" ht="10.5" customHeight="1">
-      <c r="A157" s="33">
-        <v>433.0</v>
-      </c>
-      <c r="B157" s="33" t="s">
+      <c r="X162" s="50"/>
+      <c r="Y162" s="50"/>
+      <c r="Z162" s="50"/>
+    </row>
+    <row r="163" ht="10.5" customHeight="1">
+      <c r="A163" s="42">
+        <v>443.0</v>
+      </c>
+      <c r="B163" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C157" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D157" s="33" t="s">
-        <v>361</v>
-      </c>
-      <c r="E157" s="34" t="s">
-        <v>362</v>
-      </c>
-      <c r="F157" s="36"/>
-      <c r="G157" s="36"/>
-      <c r="H157" s="36"/>
-      <c r="I157" s="41"/>
-      <c r="J157" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="K157" s="44" t="s">
-        <v>363</v>
-      </c>
-      <c r="L157" s="37"/>
-      <c r="M157" s="37"/>
-      <c r="N157" s="37"/>
-      <c r="O157" s="37"/>
-      <c r="P157" s="37"/>
-      <c r="Q157" s="37"/>
-      <c r="R157" s="37"/>
-      <c r="S157" s="37"/>
-      <c r="T157" s="37"/>
-      <c r="U157" s="38"/>
-      <c r="V157" s="39"/>
-      <c r="W157" s="37" t="s">
+      <c r="C163" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D163" s="42" t="s">
+        <v>379</v>
+      </c>
+      <c r="E163" s="39" t="s">
+        <v>380</v>
+      </c>
+      <c r="F163" s="51"/>
+      <c r="G163" s="51"/>
+      <c r="H163" s="51"/>
+      <c r="I163" s="52"/>
+      <c r="J163" s="54" t="s">
+        <v>343</v>
+      </c>
+      <c r="K163" s="46" t="s">
+        <v>369</v>
+      </c>
+      <c r="L163" s="47"/>
+      <c r="M163" s="47"/>
+      <c r="N163" s="47"/>
+      <c r="O163" s="47"/>
+      <c r="P163" s="47"/>
+      <c r="Q163" s="47"/>
+      <c r="R163" s="47"/>
+      <c r="S163" s="47"/>
+      <c r="T163" s="47"/>
+      <c r="U163" s="48"/>
+      <c r="V163" s="49"/>
+      <c r="W163" s="46" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="158" ht="10.5" customHeight="1">
-      <c r="A158" s="33">
-        <v>434.0</v>
-      </c>
-      <c r="B158" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="C158" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D158" s="33" t="s">
-        <v>364</v>
-      </c>
-      <c r="E158" s="34" t="s">
-        <v>365</v>
-      </c>
-      <c r="F158" s="36"/>
-      <c r="G158" s="42"/>
-      <c r="H158" s="42"/>
-      <c r="I158" s="43"/>
-      <c r="J158" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="K158" s="44" t="s">
-        <v>363</v>
-      </c>
-      <c r="L158" s="37"/>
-      <c r="M158" s="44"/>
-      <c r="N158" s="44"/>
-      <c r="O158" s="44"/>
-      <c r="P158" s="37"/>
-      <c r="Q158" s="37"/>
-      <c r="R158" s="37"/>
-      <c r="S158" s="37"/>
-      <c r="T158" s="44" t="s">
-        <v>353</v>
-      </c>
-      <c r="U158" s="38"/>
-      <c r="V158" s="39"/>
-      <c r="W158" s="37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="159" ht="10.5" customHeight="1">
-      <c r="A159" s="33">
-        <v>435.0</v>
-      </c>
-      <c r="B159" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="C159" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D159" s="33" t="s">
-        <v>366</v>
-      </c>
-      <c r="E159" s="34" t="s">
-        <v>367</v>
-      </c>
-      <c r="F159" s="36">
-        <v>45805.0</v>
-      </c>
-      <c r="G159" s="42">
-        <v>1.748438752E12</v>
-      </c>
-      <c r="H159" s="42" t="s">
-        <v>368</v>
-      </c>
-      <c r="I159" s="43" t="s">
-        <v>369</v>
-      </c>
-      <c r="J159" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="K159" s="37"/>
-      <c r="L159" s="37"/>
-      <c r="M159" s="44"/>
-      <c r="N159" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="O159" s="44" t="s">
-        <v>370</v>
-      </c>
-      <c r="P159" s="37"/>
-      <c r="Q159" s="37"/>
-      <c r="R159" s="37"/>
-      <c r="S159" s="37"/>
-      <c r="T159" s="44" t="s">
-        <v>353</v>
-      </c>
-      <c r="U159" s="38"/>
-      <c r="V159" s="39"/>
-      <c r="W159" s="37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="160" ht="10.5" customHeight="1">
-      <c r="A160" s="33">
-        <v>437.0</v>
-      </c>
-      <c r="B160" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="C160" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D160" s="33" t="s">
-        <v>371</v>
-      </c>
-      <c r="E160" s="34" t="s">
-        <v>372</v>
-      </c>
-      <c r="F160" s="45"/>
-      <c r="G160" s="42"/>
-      <c r="H160" s="42"/>
-      <c r="I160" s="43"/>
-      <c r="J160" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="K160" s="44" t="s">
-        <v>373</v>
-      </c>
-      <c r="L160" s="37"/>
-      <c r="M160" s="44"/>
-      <c r="N160" s="44"/>
-      <c r="O160" s="44"/>
-      <c r="P160" s="37"/>
-      <c r="Q160" s="37"/>
-      <c r="R160" s="37"/>
-      <c r="S160" s="37"/>
-      <c r="T160" s="44"/>
-      <c r="U160" s="38"/>
-      <c r="V160" s="39"/>
-      <c r="W160" s="37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="161" ht="10.5" customHeight="1">
-      <c r="A161" s="33">
-        <v>438.0</v>
-      </c>
-      <c r="B161" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="C161" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D161" s="33" t="s">
-        <v>374</v>
-      </c>
-      <c r="E161" s="34" t="s">
-        <v>375</v>
-      </c>
-      <c r="F161" s="36"/>
-      <c r="G161" s="42"/>
-      <c r="H161" s="42"/>
-      <c r="I161" s="43"/>
-      <c r="J161" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="K161" s="44" t="s">
-        <v>373</v>
-      </c>
-      <c r="L161" s="37"/>
-      <c r="M161" s="44"/>
-      <c r="N161" s="44"/>
-      <c r="O161" s="44"/>
-      <c r="P161" s="44"/>
-      <c r="Q161" s="37"/>
-      <c r="R161" s="37"/>
-      <c r="S161" s="37"/>
-      <c r="T161" s="44"/>
-      <c r="U161" s="38"/>
-      <c r="V161" s="39"/>
-      <c r="W161" s="37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="162" ht="10.5" customHeight="1">
-      <c r="A162" s="33">
-        <v>440.0</v>
-      </c>
-      <c r="B162" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="C162" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D162" s="33" t="s">
-        <v>376</v>
-      </c>
-      <c r="E162" s="34" t="s">
-        <v>377</v>
-      </c>
-      <c r="F162" s="36"/>
-      <c r="G162" s="36"/>
-      <c r="H162" s="36"/>
-      <c r="I162" s="41"/>
-      <c r="J162" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="K162" s="44" t="s">
-        <v>373</v>
-      </c>
-      <c r="L162" s="37"/>
-      <c r="M162" s="37"/>
-      <c r="N162" s="37"/>
-      <c r="O162" s="37"/>
-      <c r="P162" s="37"/>
-      <c r="Q162" s="37"/>
-      <c r="R162" s="37"/>
-      <c r="S162" s="37"/>
-      <c r="T162" s="37"/>
-      <c r="U162" s="38"/>
-      <c r="V162" s="39"/>
-      <c r="W162" s="37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="163" ht="10.5" customHeight="1">
-      <c r="A163" s="33">
-        <v>441.0</v>
-      </c>
-      <c r="B163" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="C163" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D163" s="33" t="s">
-        <v>378</v>
-      </c>
-      <c r="E163" s="34" t="s">
-        <v>379</v>
-      </c>
-      <c r="F163" s="36"/>
-      <c r="G163" s="36"/>
-      <c r="H163" s="36"/>
-      <c r="I163" s="41"/>
-      <c r="J163" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="K163" s="44" t="s">
-        <v>373</v>
-      </c>
-      <c r="L163" s="37"/>
-      <c r="M163" s="37"/>
-      <c r="N163" s="37"/>
-      <c r="O163" s="37"/>
-      <c r="P163" s="37"/>
-      <c r="Q163" s="37"/>
-      <c r="R163" s="37"/>
-      <c r="S163" s="37"/>
-      <c r="T163" s="37"/>
-      <c r="U163" s="38"/>
-      <c r="V163" s="39"/>
-      <c r="W163" s="37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="164" ht="10.5" customHeight="1">
+      <c r="X163" s="50"/>
+      <c r="Y163" s="50"/>
+      <c r="Z163" s="50"/>
+    </row>
+    <row r="164" ht="10.5" hidden="1" customHeight="1">
       <c r="A164" s="33">
-        <v>442.0</v>
+        <v>444.0</v>
       </c>
       <c r="B164" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C164" s="40" t="s">
-        <v>331</v>
+        <v>57</v>
       </c>
       <c r="D164" s="33" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E164" s="34" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="F164" s="36"/>
       <c r="G164" s="36"/>
       <c r="H164" s="36"/>
       <c r="I164" s="41"/>
-      <c r="J164" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="K164" s="44" t="s">
-        <v>382</v>
-      </c>
+      <c r="J164" s="37"/>
+      <c r="K164" s="37"/>
       <c r="L164" s="37"/>
       <c r="M164" s="37"/>
       <c r="N164" s="37"/>
@@ -11473,18 +11546,18 @@
       <c r="U164" s="38"/>
       <c r="V164" s="39"/>
       <c r="W164" s="37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="165" ht="10.5" customHeight="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="165" ht="10.5" hidden="1" customHeight="1">
       <c r="A165" s="33">
-        <v>443.0</v>
+        <v>445.0</v>
       </c>
       <c r="B165" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C165" s="40" t="s">
-        <v>331</v>
+        <v>57</v>
       </c>
       <c r="D165" s="33" t="s">
         <v>383</v>
@@ -11496,12 +11569,8 @@
       <c r="G165" s="36"/>
       <c r="H165" s="36"/>
       <c r="I165" s="41"/>
-      <c r="J165" s="46" t="s">
-        <v>347</v>
-      </c>
-      <c r="K165" s="44" t="s">
-        <v>373</v>
-      </c>
+      <c r="J165" s="37"/>
+      <c r="K165" s="37"/>
       <c r="L165" s="37"/>
       <c r="M165" s="37"/>
       <c r="N165" s="37"/>
@@ -11514,18 +11583,18 @@
       <c r="U165" s="38"/>
       <c r="V165" s="39"/>
       <c r="W165" s="37" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="166" ht="10.5" hidden="1" customHeight="1">
       <c r="A166" s="33">
-        <v>444.0</v>
+        <v>448.0</v>
       </c>
       <c r="B166" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C166" s="40" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D166" s="33" t="s">
         <v>385</v>
@@ -11556,13 +11625,13 @@
     </row>
     <row r="167" ht="10.5" hidden="1" customHeight="1">
       <c r="A167" s="33">
-        <v>445.0</v>
+        <v>449.0</v>
       </c>
       <c r="B167" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C167" s="40" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D167" s="33" t="s">
         <v>387</v>
@@ -11593,13 +11662,13 @@
     </row>
     <row r="168" ht="10.5" hidden="1" customHeight="1">
       <c r="A168" s="33">
-        <v>446.0</v>
+        <v>450.0</v>
       </c>
       <c r="B168" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C168" s="40" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D168" s="33" t="s">
         <v>389</v>
@@ -11630,13 +11699,13 @@
     </row>
     <row r="169" ht="10.5" hidden="1" customHeight="1">
       <c r="A169" s="33">
-        <v>447.0</v>
+        <v>451.0</v>
       </c>
       <c r="B169" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C169" s="40" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D169" s="33" t="s">
         <v>391</v>
@@ -11667,13 +11736,13 @@
     </row>
     <row r="170" ht="10.5" hidden="1" customHeight="1">
       <c r="A170" s="33">
-        <v>448.0</v>
+        <v>452.0</v>
       </c>
       <c r="B170" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C170" s="40" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="D170" s="33" t="s">
         <v>393</v>
@@ -11702,15 +11771,15 @@
         <v>50</v>
       </c>
     </row>
-    <row r="171" ht="10.5" hidden="1" customHeight="1">
+    <row r="171" ht="14.25" hidden="1" customHeight="1">
       <c r="A171" s="33">
-        <v>449.0</v>
+        <v>454.0</v>
       </c>
       <c r="B171" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C171" s="40" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D171" s="33" t="s">
         <v>395</v>
@@ -11739,15 +11808,15 @@
         <v>50</v>
       </c>
     </row>
-    <row r="172" ht="10.5" hidden="1" customHeight="1">
+    <row r="172" ht="14.25" hidden="1" customHeight="1">
       <c r="A172" s="33">
-        <v>450.0</v>
+        <v>455.0</v>
       </c>
       <c r="B172" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C172" s="40" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="D172" s="33" t="s">
         <v>397</v>
@@ -11776,15 +11845,15 @@
         <v>50</v>
       </c>
     </row>
-    <row r="173" ht="10.5" hidden="1" customHeight="1">
+    <row r="173" ht="14.25" hidden="1" customHeight="1">
       <c r="A173" s="33">
-        <v>451.0</v>
+        <v>456.0</v>
       </c>
       <c r="B173" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C173" s="40" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D173" s="33" t="s">
         <v>399</v>
@@ -11815,13 +11884,13 @@
     </row>
     <row r="174" ht="10.5" hidden="1" customHeight="1">
       <c r="A174" s="33">
-        <v>452.0</v>
+        <v>457.0</v>
       </c>
       <c r="B174" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C174" s="40" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="D174" s="33" t="s">
         <v>401</v>
@@ -11850,15 +11919,15 @@
         <v>50</v>
       </c>
     </row>
-    <row r="175" ht="14.25" hidden="1" customHeight="1">
+    <row r="175" ht="10.5" hidden="1" customHeight="1">
       <c r="A175" s="33">
-        <v>454.0</v>
+        <v>458.0</v>
       </c>
       <c r="B175" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C175" s="40" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D175" s="33" t="s">
         <v>403</v>
@@ -11889,13 +11958,13 @@
     </row>
     <row r="176" ht="14.25" hidden="1" customHeight="1">
       <c r="A176" s="33">
-        <v>455.0</v>
+        <v>459.0</v>
       </c>
       <c r="B176" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C176" s="40" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D176" s="33" t="s">
         <v>405</v>
@@ -11924,234 +11993,237 @@
         <v>50</v>
       </c>
     </row>
-    <row r="177" ht="14.25" hidden="1" customHeight="1">
-      <c r="A177" s="33">
-        <v>456.0</v>
-      </c>
-      <c r="B177" s="33" t="s">
+    <row r="177" ht="14.25" customHeight="1">
+      <c r="A177" s="42">
+        <v>460.0</v>
+      </c>
+      <c r="B177" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C177" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="D177" s="33" t="s">
+      <c r="C177" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D177" s="42" t="s">
         <v>407</v>
       </c>
-      <c r="E177" s="34" t="s">
+      <c r="E177" s="39" t="s">
         <v>408</v>
       </c>
-      <c r="F177" s="36"/>
-      <c r="G177" s="36"/>
-      <c r="H177" s="36"/>
-      <c r="I177" s="41"/>
-      <c r="J177" s="37"/>
-      <c r="K177" s="37"/>
-      <c r="L177" s="37"/>
-      <c r="M177" s="37"/>
-      <c r="N177" s="37"/>
-      <c r="O177" s="37"/>
-      <c r="P177" s="37"/>
-      <c r="Q177" s="37"/>
-      <c r="R177" s="37"/>
-      <c r="S177" s="37"/>
-      <c r="T177" s="37"/>
-      <c r="U177" s="38"/>
-      <c r="V177" s="39"/>
-      <c r="W177" s="37" t="s">
+      <c r="F177" s="44">
+        <v>45805.0</v>
+      </c>
+      <c r="G177" s="44">
+        <v>1.748428967E12</v>
+      </c>
+      <c r="H177" s="44" t="s">
+        <v>409</v>
+      </c>
+      <c r="I177" s="45" t="s">
+        <v>410</v>
+      </c>
+      <c r="J177" s="46" t="s">
+        <v>411</v>
+      </c>
+      <c r="K177" s="47"/>
+      <c r="L177" s="47"/>
+      <c r="M177" s="47"/>
+      <c r="N177" s="47"/>
+      <c r="O177" s="47"/>
+      <c r="P177" s="47"/>
+      <c r="Q177" s="47"/>
+      <c r="R177" s="47"/>
+      <c r="S177" s="47"/>
+      <c r="T177" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="U177" s="48"/>
+      <c r="V177" s="49"/>
+      <c r="W177" s="46" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="178" ht="10.5" hidden="1" customHeight="1">
+      <c r="X177" s="50"/>
+      <c r="Y177" s="50"/>
+      <c r="Z177" s="50"/>
+    </row>
+    <row r="178" ht="14.25" hidden="1" customHeight="1">
       <c r="A178" s="33">
-        <v>457.0</v>
+        <v>461.0</v>
       </c>
       <c r="B178" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C178" s="40" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D178" s="33" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="E178" s="34" t="s">
-        <v>410</v>
-      </c>
-      <c r="F178" s="36"/>
-      <c r="G178" s="36"/>
-      <c r="H178" s="36"/>
-      <c r="I178" s="41"/>
+        <v>413</v>
+      </c>
+      <c r="F178" s="33"/>
+      <c r="G178" s="33"/>
+      <c r="H178" s="33"/>
+      <c r="I178" s="33"/>
       <c r="J178" s="37"/>
       <c r="K178" s="37"/>
-      <c r="L178" s="37"/>
+      <c r="L178" s="33"/>
       <c r="M178" s="37"/>
       <c r="N178" s="37"/>
-      <c r="O178" s="37"/>
+      <c r="O178" s="33"/>
       <c r="P178" s="37"/>
       <c r="Q178" s="37"/>
       <c r="R178" s="37"/>
-      <c r="S178" s="37"/>
+      <c r="S178" s="33"/>
       <c r="T178" s="37"/>
-      <c r="U178" s="38"/>
-      <c r="V178" s="39"/>
-      <c r="W178" s="37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="179" ht="10.5" hidden="1" customHeight="1">
+      <c r="U178" s="33"/>
+      <c r="V178" s="33"/>
+      <c r="W178" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="179" ht="14.25" hidden="1" customHeight="1">
       <c r="A179" s="33">
-        <v>458.0</v>
+        <v>462.0</v>
       </c>
       <c r="B179" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C179" s="40" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D179" s="33" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="E179" s="34" t="s">
-        <v>412</v>
-      </c>
-      <c r="F179" s="36"/>
-      <c r="G179" s="36"/>
-      <c r="H179" s="36"/>
-      <c r="I179" s="41"/>
+        <v>415</v>
+      </c>
+      <c r="F179" s="33"/>
+      <c r="G179" s="33"/>
+      <c r="H179" s="33"/>
+      <c r="I179" s="33"/>
       <c r="J179" s="37"/>
       <c r="K179" s="37"/>
-      <c r="L179" s="37"/>
+      <c r="L179" s="33"/>
       <c r="M179" s="37"/>
       <c r="N179" s="37"/>
-      <c r="O179" s="37"/>
+      <c r="O179" s="33"/>
       <c r="P179" s="37"/>
       <c r="Q179" s="37"/>
       <c r="R179" s="37"/>
-      <c r="S179" s="37"/>
+      <c r="S179" s="33"/>
       <c r="T179" s="37"/>
-      <c r="U179" s="38"/>
-      <c r="V179" s="39"/>
-      <c r="W179" s="37" t="s">
-        <v>50</v>
+      <c r="U179" s="33"/>
+      <c r="V179" s="33"/>
+      <c r="W179" s="33" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="180" ht="14.25" hidden="1" customHeight="1">
       <c r="A180" s="33">
-        <v>459.0</v>
+        <v>463.0</v>
       </c>
       <c r="B180" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C180" s="40" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D180" s="33" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="E180" s="34" t="s">
-        <v>414</v>
-      </c>
-      <c r="F180" s="36"/>
-      <c r="G180" s="36"/>
-      <c r="H180" s="36"/>
-      <c r="I180" s="41"/>
+        <v>417</v>
+      </c>
+      <c r="F180" s="33"/>
+      <c r="G180" s="33"/>
+      <c r="H180" s="33"/>
+      <c r="I180" s="33"/>
       <c r="J180" s="37"/>
       <c r="K180" s="37"/>
-      <c r="L180" s="37"/>
+      <c r="L180" s="33"/>
       <c r="M180" s="37"/>
       <c r="N180" s="37"/>
-      <c r="O180" s="37"/>
+      <c r="O180" s="33"/>
       <c r="P180" s="37"/>
       <c r="Q180" s="37"/>
       <c r="R180" s="37"/>
-      <c r="S180" s="37"/>
+      <c r="S180" s="33"/>
       <c r="T180" s="37"/>
-      <c r="U180" s="38"/>
-      <c r="V180" s="39"/>
-      <c r="W180" s="37" t="s">
-        <v>50</v>
+      <c r="U180" s="33"/>
+      <c r="V180" s="33"/>
+      <c r="W180" s="33" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="181" ht="14.25" hidden="1" customHeight="1">
       <c r="A181" s="33">
-        <v>460.0</v>
+        <v>464.0</v>
       </c>
       <c r="B181" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C181" s="40" t="s">
-        <v>331</v>
+        <v>66</v>
       </c>
       <c r="D181" s="33" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="E181" s="34" t="s">
-        <v>416</v>
-      </c>
-      <c r="F181" s="36">
-        <v>45805.0</v>
-      </c>
-      <c r="G181" s="42">
-        <v>1.748428967E12</v>
-      </c>
-      <c r="H181" s="42" t="s">
-        <v>417</v>
-      </c>
-      <c r="I181" s="43" t="s">
-        <v>418</v>
-      </c>
-      <c r="J181" s="44" t="s">
         <v>419</v>
       </c>
+      <c r="F181" s="33"/>
+      <c r="G181" s="33"/>
+      <c r="H181" s="33"/>
+      <c r="I181" s="33"/>
+      <c r="J181" s="37"/>
       <c r="K181" s="37"/>
-      <c r="L181" s="37"/>
+      <c r="L181" s="33"/>
       <c r="M181" s="37"/>
       <c r="N181" s="37"/>
-      <c r="O181" s="37"/>
+      <c r="O181" s="33"/>
       <c r="P181" s="37"/>
       <c r="Q181" s="37"/>
       <c r="R181" s="37"/>
-      <c r="S181" s="37"/>
-      <c r="T181" s="44" t="s">
-        <v>336</v>
-      </c>
-      <c r="U181" s="38"/>
-      <c r="V181" s="39"/>
-      <c r="W181" s="37" t="s">
-        <v>50</v>
+      <c r="S181" s="33"/>
+      <c r="T181" s="37"/>
+      <c r="U181" s="33"/>
+      <c r="V181" s="33"/>
+      <c r="W181" s="33" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="182" ht="14.25" hidden="1" customHeight="1">
       <c r="A182" s="33">
-        <v>461.0</v>
+        <v>465.0</v>
       </c>
       <c r="B182" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C182" s="40" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D182" s="33" t="s">
         <v>420</v>
       </c>
-      <c r="E182" s="33" t="s">
+      <c r="E182" s="34" t="s">
         <v>421</v>
       </c>
       <c r="F182" s="33"/>
       <c r="G182" s="33"/>
       <c r="H182" s="33"/>
       <c r="I182" s="33"/>
-      <c r="J182" s="33"/>
-      <c r="K182" s="33"/>
+      <c r="J182" s="37"/>
+      <c r="K182" s="37"/>
       <c r="L182" s="33"/>
-      <c r="M182" s="33"/>
-      <c r="N182" s="33"/>
+      <c r="M182" s="37"/>
+      <c r="N182" s="37"/>
       <c r="O182" s="33"/>
-      <c r="P182" s="33"/>
-      <c r="Q182" s="33"/>
-      <c r="R182" s="33"/>
+      <c r="P182" s="37"/>
+      <c r="Q182" s="37"/>
+      <c r="R182" s="37"/>
       <c r="S182" s="33"/>
-      <c r="T182" s="33"/>
+      <c r="T182" s="37"/>
       <c r="U182" s="33"/>
       <c r="V182" s="33"/>
       <c r="W182" s="33" t="s">
@@ -12160,35 +12232,35 @@
     </row>
     <row r="183" ht="14.25" hidden="1" customHeight="1">
       <c r="A183" s="33">
-        <v>462.0</v>
+        <v>466.0</v>
       </c>
       <c r="B183" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C183" s="40" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D183" s="33" t="s">
         <v>422</v>
       </c>
-      <c r="E183" s="37" t="s">
+      <c r="E183" s="34" t="s">
         <v>423</v>
       </c>
       <c r="F183" s="33"/>
       <c r="G183" s="33"/>
       <c r="H183" s="33"/>
       <c r="I183" s="33"/>
-      <c r="J183" s="33"/>
-      <c r="K183" s="33"/>
+      <c r="J183" s="37"/>
+      <c r="K183" s="37"/>
       <c r="L183" s="33"/>
-      <c r="M183" s="33"/>
-      <c r="N183" s="33"/>
+      <c r="M183" s="37"/>
+      <c r="N183" s="37"/>
       <c r="O183" s="33"/>
-      <c r="P183" s="33"/>
-      <c r="Q183" s="33"/>
-      <c r="R183" s="33"/>
+      <c r="P183" s="37"/>
+      <c r="Q183" s="37"/>
+      <c r="R183" s="37"/>
       <c r="S183" s="33"/>
-      <c r="T183" s="33"/>
+      <c r="T183" s="37"/>
       <c r="U183" s="33"/>
       <c r="V183" s="33"/>
       <c r="W183" s="33" t="s">
@@ -12197,35 +12269,35 @@
     </row>
     <row r="184" ht="14.25" hidden="1" customHeight="1">
       <c r="A184" s="33">
-        <v>463.0</v>
+        <v>467.0</v>
       </c>
       <c r="B184" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C184" s="40" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D184" s="33" t="s">
         <v>424</v>
       </c>
-      <c r="E184" s="37" t="s">
+      <c r="E184" s="34" t="s">
         <v>425</v>
       </c>
       <c r="F184" s="33"/>
       <c r="G184" s="33"/>
       <c r="H184" s="33"/>
       <c r="I184" s="33"/>
-      <c r="J184" s="33"/>
-      <c r="K184" s="33"/>
+      <c r="J184" s="37"/>
+      <c r="K184" s="37"/>
       <c r="L184" s="33"/>
-      <c r="M184" s="33"/>
-      <c r="N184" s="33"/>
+      <c r="M184" s="37"/>
+      <c r="N184" s="37"/>
       <c r="O184" s="33"/>
-      <c r="P184" s="33"/>
-      <c r="Q184" s="33"/>
-      <c r="R184" s="33"/>
+      <c r="P184" s="37"/>
+      <c r="Q184" s="37"/>
+      <c r="R184" s="37"/>
       <c r="S184" s="33"/>
-      <c r="T184" s="33"/>
+      <c r="T184" s="37"/>
       <c r="U184" s="33"/>
       <c r="V184" s="33"/>
       <c r="W184" s="33" t="s">
@@ -12234,13 +12306,13 @@
     </row>
     <row r="185" ht="14.25" hidden="1" customHeight="1">
       <c r="A185" s="33">
-        <v>464.0</v>
+        <v>468.0</v>
       </c>
       <c r="B185" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C185" s="40" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D185" s="33" t="s">
         <v>426</v>
@@ -12252,17 +12324,17 @@
       <c r="G185" s="33"/>
       <c r="H185" s="33"/>
       <c r="I185" s="33"/>
-      <c r="J185" s="33"/>
-      <c r="K185" s="33"/>
+      <c r="J185" s="37"/>
+      <c r="K185" s="37"/>
       <c r="L185" s="33"/>
-      <c r="M185" s="33"/>
-      <c r="N185" s="33"/>
+      <c r="M185" s="37"/>
+      <c r="N185" s="37"/>
       <c r="O185" s="33"/>
-      <c r="P185" s="33"/>
-      <c r="Q185" s="33"/>
-      <c r="R185" s="33"/>
+      <c r="P185" s="37"/>
+      <c r="Q185" s="37"/>
+      <c r="R185" s="37"/>
       <c r="S185" s="33"/>
-      <c r="T185" s="33"/>
+      <c r="T185" s="37"/>
       <c r="U185" s="33"/>
       <c r="V185" s="33"/>
       <c r="W185" s="33" t="s">
@@ -12271,13 +12343,13 @@
     </row>
     <row r="186" ht="14.25" hidden="1" customHeight="1">
       <c r="A186" s="33">
-        <v>465.0</v>
+        <v>469.0</v>
       </c>
       <c r="B186" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C186" s="40" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D186" s="33" t="s">
         <v>428</v>
@@ -12289,231 +12361,251 @@
       <c r="G186" s="33"/>
       <c r="H186" s="33"/>
       <c r="I186" s="33"/>
-      <c r="J186" s="33"/>
-      <c r="K186" s="33"/>
+      <c r="J186" s="37"/>
+      <c r="K186" s="37"/>
       <c r="L186" s="33"/>
-      <c r="M186" s="33"/>
-      <c r="N186" s="33"/>
+      <c r="M186" s="37"/>
+      <c r="N186" s="37"/>
       <c r="O186" s="33"/>
-      <c r="P186" s="33"/>
-      <c r="Q186" s="33"/>
-      <c r="R186" s="33"/>
+      <c r="P186" s="37"/>
+      <c r="Q186" s="37"/>
+      <c r="R186" s="37"/>
       <c r="S186" s="33"/>
-      <c r="T186" s="33"/>
+      <c r="T186" s="37"/>
       <c r="U186" s="33"/>
       <c r="V186" s="33"/>
       <c r="W186" s="33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="187" ht="14.25" hidden="1" customHeight="1">
-      <c r="A187" s="33">
-        <v>466.0</v>
-      </c>
-      <c r="B187" s="33" t="s">
+    <row r="187" ht="14.25" customHeight="1">
+      <c r="A187" s="42">
+        <v>470.0</v>
+      </c>
+      <c r="B187" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C187" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D187" s="33" t="s">
+      <c r="C187" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D187" s="42" t="s">
         <v>430</v>
       </c>
-      <c r="E187" s="34" t="s">
+      <c r="E187" s="46" t="s">
         <v>431</v>
       </c>
-      <c r="F187" s="33"/>
-      <c r="G187" s="33"/>
-      <c r="H187" s="33"/>
-      <c r="I187" s="33"/>
-      <c r="J187" s="33"/>
-      <c r="K187" s="33"/>
-      <c r="L187" s="33"/>
-      <c r="M187" s="33"/>
-      <c r="N187" s="33"/>
-      <c r="O187" s="33"/>
-      <c r="P187" s="33"/>
-      <c r="Q187" s="33"/>
-      <c r="R187" s="33"/>
-      <c r="S187" s="33"/>
-      <c r="T187" s="33"/>
-      <c r="U187" s="33"/>
-      <c r="V187" s="33"/>
-      <c r="W187" s="33" t="s">
+      <c r="F187" s="47"/>
+      <c r="G187" s="47"/>
+      <c r="H187" s="47"/>
+      <c r="I187" s="47"/>
+      <c r="J187" s="42" t="s">
+        <v>343</v>
+      </c>
+      <c r="K187" s="42" t="s">
+        <v>369</v>
+      </c>
+      <c r="L187" s="47"/>
+      <c r="M187" s="47"/>
+      <c r="N187" s="47"/>
+      <c r="O187" s="47"/>
+      <c r="P187" s="47"/>
+      <c r="Q187" s="47"/>
+      <c r="R187" s="47"/>
+      <c r="S187" s="47"/>
+      <c r="T187" s="47"/>
+      <c r="U187" s="47"/>
+      <c r="V187" s="47"/>
+      <c r="W187" s="42" t="s">
         <v>53</v>
       </c>
+      <c r="X187" s="50"/>
+      <c r="Y187" s="50"/>
+      <c r="Z187" s="50"/>
     </row>
     <row r="188" ht="14.25" hidden="1" customHeight="1">
       <c r="A188" s="33">
-        <v>467.0</v>
+        <v>471.0</v>
       </c>
       <c r="B188" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C188" s="40" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D188" s="33" t="s">
         <v>432</v>
       </c>
-      <c r="E188" s="37" t="s">
+      <c r="E188" s="34" t="s">
         <v>433</v>
       </c>
-      <c r="F188" s="33"/>
-      <c r="G188" s="33"/>
-      <c r="H188" s="33"/>
-      <c r="I188" s="33"/>
-      <c r="J188" s="33"/>
-      <c r="K188" s="33"/>
-      <c r="L188" s="33"/>
-      <c r="M188" s="33"/>
-      <c r="N188" s="33"/>
-      <c r="O188" s="33"/>
-      <c r="P188" s="33"/>
-      <c r="Q188" s="33"/>
-      <c r="R188" s="33"/>
-      <c r="S188" s="33"/>
-      <c r="T188" s="33"/>
-      <c r="U188" s="33"/>
-      <c r="V188" s="33"/>
-      <c r="W188" s="33" t="s">
-        <v>53</v>
+      <c r="F188" s="36"/>
+      <c r="G188" s="36"/>
+      <c r="H188" s="36"/>
+      <c r="I188" s="41"/>
+      <c r="J188" s="37"/>
+      <c r="K188" s="37"/>
+      <c r="L188" s="37"/>
+      <c r="M188" s="37"/>
+      <c r="N188" s="37"/>
+      <c r="O188" s="37"/>
+      <c r="P188" s="37"/>
+      <c r="Q188" s="37"/>
+      <c r="R188" s="37"/>
+      <c r="S188" s="37"/>
+      <c r="T188" s="37"/>
+      <c r="U188" s="38"/>
+      <c r="V188" s="39"/>
+      <c r="W188" s="37" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="189" ht="14.25" hidden="1" customHeight="1">
       <c r="A189" s="33">
-        <v>468.0</v>
+        <v>472.0</v>
       </c>
       <c r="B189" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C189" s="40" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D189" s="33" t="s">
         <v>434</v>
       </c>
-      <c r="E189" s="37" t="s">
+      <c r="E189" s="34" t="s">
         <v>435</v>
       </c>
-      <c r="F189" s="33"/>
-      <c r="G189" s="33"/>
-      <c r="H189" s="33"/>
-      <c r="I189" s="33"/>
-      <c r="J189" s="33"/>
-      <c r="K189" s="33"/>
-      <c r="L189" s="33"/>
-      <c r="M189" s="33"/>
-      <c r="N189" s="33"/>
-      <c r="O189" s="33"/>
-      <c r="P189" s="33"/>
-      <c r="Q189" s="33"/>
-      <c r="R189" s="33"/>
-      <c r="S189" s="33"/>
-      <c r="T189" s="33"/>
-      <c r="U189" s="33"/>
-      <c r="V189" s="33"/>
-      <c r="W189" s="33" t="s">
-        <v>53</v>
+      <c r="F189" s="36"/>
+      <c r="G189" s="36"/>
+      <c r="H189" s="36"/>
+      <c r="I189" s="41"/>
+      <c r="J189" s="37"/>
+      <c r="K189" s="37"/>
+      <c r="L189" s="37"/>
+      <c r="M189" s="37"/>
+      <c r="N189" s="37"/>
+      <c r="O189" s="37"/>
+      <c r="P189" s="37"/>
+      <c r="Q189" s="37"/>
+      <c r="R189" s="37"/>
+      <c r="S189" s="37"/>
+      <c r="T189" s="37"/>
+      <c r="U189" s="38"/>
+      <c r="V189" s="39"/>
+      <c r="W189" s="37" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="190" ht="14.25" hidden="1" customHeight="1">
       <c r="A190" s="33">
-        <v>469.0</v>
+        <v>473.0</v>
       </c>
       <c r="B190" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C190" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="D190" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D190" s="40" t="s">
         <v>436</v>
       </c>
-      <c r="E190" s="37" t="s">
+      <c r="E190" s="34" t="s">
         <v>437</v>
       </c>
-      <c r="F190" s="33"/>
-      <c r="G190" s="33"/>
-      <c r="H190" s="33"/>
-      <c r="I190" s="33"/>
-      <c r="J190" s="33"/>
-      <c r="K190" s="33"/>
-      <c r="L190" s="33"/>
-      <c r="M190" s="33"/>
-      <c r="N190" s="33"/>
-      <c r="O190" s="33"/>
-      <c r="P190" s="33"/>
-      <c r="Q190" s="33"/>
-      <c r="R190" s="33"/>
-      <c r="S190" s="33"/>
-      <c r="T190" s="33"/>
-      <c r="U190" s="33"/>
-      <c r="V190" s="33"/>
-      <c r="W190" s="33" t="s">
+      <c r="F190" s="36"/>
+      <c r="G190" s="36"/>
+      <c r="H190" s="36"/>
+      <c r="I190" s="41"/>
+      <c r="J190" s="37"/>
+      <c r="K190" s="37"/>
+      <c r="L190" s="37"/>
+      <c r="M190" s="37"/>
+      <c r="N190" s="37"/>
+      <c r="O190" s="37"/>
+      <c r="P190" s="37"/>
+      <c r="Q190" s="37"/>
+      <c r="R190" s="37"/>
+      <c r="S190" s="37"/>
+      <c r="T190" s="37"/>
+      <c r="U190" s="38"/>
+      <c r="V190" s="39"/>
+      <c r="W190" s="37" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="191" ht="14.25" customHeight="1">
+    <row r="191" ht="14.25" hidden="1" customHeight="1">
       <c r="A191" s="33">
-        <v>470.0</v>
+        <v>474.0</v>
       </c>
       <c r="B191" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C191" s="40" t="s">
-        <v>331</v>
+        <v>60</v>
       </c>
       <c r="D191" s="33" t="s">
         <v>438</v>
       </c>
-      <c r="E191" s="37" t="s">
+      <c r="E191" s="34" t="s">
         <v>439</v>
       </c>
-      <c r="F191" s="33"/>
-      <c r="G191" s="33"/>
-      <c r="H191" s="33"/>
-      <c r="I191" s="33"/>
-      <c r="J191" s="47" t="s">
-        <v>347</v>
-      </c>
-      <c r="K191" s="47" t="s">
-        <v>373</v>
-      </c>
-      <c r="L191" s="33"/>
-      <c r="M191" s="33"/>
-      <c r="N191" s="33"/>
-      <c r="O191" s="33"/>
-      <c r="P191" s="33"/>
-      <c r="Q191" s="33"/>
-      <c r="R191" s="33"/>
-      <c r="S191" s="33"/>
-      <c r="T191" s="33"/>
-      <c r="U191" s="33"/>
-      <c r="V191" s="33"/>
-      <c r="W191" s="33" t="s">
+      <c r="F191" s="36"/>
+      <c r="G191" s="36"/>
+      <c r="H191" s="36"/>
+      <c r="I191" s="41"/>
+      <c r="J191" s="37"/>
+      <c r="K191" s="37"/>
+      <c r="L191" s="37"/>
+      <c r="M191" s="37"/>
+      <c r="N191" s="37"/>
+      <c r="O191" s="37"/>
+      <c r="P191" s="37"/>
+      <c r="Q191" s="37"/>
+      <c r="R191" s="37"/>
+      <c r="S191" s="37"/>
+      <c r="T191" s="37"/>
+      <c r="U191" s="38"/>
+      <c r="V191" s="39"/>
+      <c r="W191" s="37" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="192" ht="14.25" customHeight="1">
-      <c r="F192" s="11"/>
-      <c r="G192" s="11"/>
-      <c r="H192" s="11"/>
-      <c r="I192" s="11"/>
-      <c r="J192" s="12"/>
-      <c r="K192" s="12"/>
-      <c r="L192" s="12"/>
-      <c r="M192" s="12"/>
-      <c r="N192" s="12"/>
-      <c r="O192" s="12"/>
-      <c r="P192" s="12"/>
-      <c r="Q192" s="12"/>
-      <c r="R192" s="12"/>
-      <c r="S192" s="12"/>
-      <c r="T192" s="12"/>
-      <c r="U192" s="13"/>
-      <c r="V192" s="2"/>
-      <c r="W192" s="14"/>
+    <row r="192" ht="14.25" hidden="1" customHeight="1">
+      <c r="A192" s="33">
+        <v>475.0</v>
+      </c>
+      <c r="B192" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C192" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D192" s="33" t="s">
+        <v>440</v>
+      </c>
+      <c r="E192" s="34" t="s">
+        <v>441</v>
+      </c>
+      <c r="F192" s="36"/>
+      <c r="G192" s="36"/>
+      <c r="H192" s="36"/>
+      <c r="I192" s="41"/>
+      <c r="J192" s="37"/>
+      <c r="K192" s="37"/>
+      <c r="L192" s="37"/>
+      <c r="M192" s="37"/>
+      <c r="N192" s="37"/>
+      <c r="O192" s="37"/>
+      <c r="P192" s="37"/>
+      <c r="Q192" s="37"/>
+      <c r="R192" s="37"/>
+      <c r="S192" s="37"/>
+      <c r="T192" s="37"/>
+      <c r="U192" s="38"/>
+      <c r="V192" s="39"/>
+      <c r="W192" s="37" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="193" ht="14.25" customHeight="1">
       <c r="F193" s="11"/>
@@ -15276,84 +15368,16 @@
       <c r="W330" s="14"/>
     </row>
     <row r="331" ht="14.25" customHeight="1">
-      <c r="F331" s="11"/>
-      <c r="G331" s="11"/>
-      <c r="H331" s="11"/>
-      <c r="I331" s="11"/>
-      <c r="J331" s="12"/>
-      <c r="K331" s="12"/>
-      <c r="L331" s="12"/>
-      <c r="M331" s="12"/>
-      <c r="N331" s="12"/>
-      <c r="O331" s="12"/>
-      <c r="P331" s="12"/>
-      <c r="Q331" s="12"/>
-      <c r="R331" s="12"/>
-      <c r="S331" s="12"/>
-      <c r="T331" s="12"/>
-      <c r="U331" s="13"/>
-      <c r="V331" s="2"/>
-      <c r="W331" s="14"/>
+      <c r="W331" s="12"/>
     </row>
     <row r="332" ht="14.25" customHeight="1">
-      <c r="F332" s="11"/>
-      <c r="G332" s="11"/>
-      <c r="H332" s="11"/>
-      <c r="I332" s="11"/>
-      <c r="J332" s="12"/>
-      <c r="K332" s="12"/>
-      <c r="L332" s="12"/>
-      <c r="M332" s="12"/>
-      <c r="N332" s="12"/>
-      <c r="O332" s="12"/>
-      <c r="P332" s="12"/>
-      <c r="Q332" s="12"/>
-      <c r="R332" s="12"/>
-      <c r="S332" s="12"/>
-      <c r="T332" s="12"/>
-      <c r="U332" s="13"/>
-      <c r="V332" s="2"/>
-      <c r="W332" s="14"/>
+      <c r="W332" s="12"/>
     </row>
     <row r="333" ht="14.25" customHeight="1">
-      <c r="F333" s="11"/>
-      <c r="G333" s="11"/>
-      <c r="H333" s="11"/>
-      <c r="I333" s="11"/>
-      <c r="J333" s="12"/>
-      <c r="K333" s="12"/>
-      <c r="L333" s="12"/>
-      <c r="M333" s="12"/>
-      <c r="N333" s="12"/>
-      <c r="O333" s="12"/>
-      <c r="P333" s="12"/>
-      <c r="Q333" s="12"/>
-      <c r="R333" s="12"/>
-      <c r="S333" s="12"/>
-      <c r="T333" s="12"/>
-      <c r="U333" s="13"/>
-      <c r="V333" s="2"/>
-      <c r="W333" s="14"/>
+      <c r="W333" s="12"/>
     </row>
     <row r="334" ht="14.25" customHeight="1">
-      <c r="F334" s="11"/>
-      <c r="G334" s="11"/>
-      <c r="H334" s="11"/>
-      <c r="I334" s="11"/>
-      <c r="J334" s="12"/>
-      <c r="K334" s="12"/>
-      <c r="L334" s="12"/>
-      <c r="M334" s="12"/>
-      <c r="N334" s="12"/>
-      <c r="O334" s="12"/>
-      <c r="P334" s="12"/>
-      <c r="Q334" s="12"/>
-      <c r="R334" s="12"/>
-      <c r="S334" s="12"/>
-      <c r="T334" s="12"/>
-      <c r="U334" s="13"/>
-      <c r="V334" s="2"/>
-      <c r="W334" s="14"/>
+      <c r="W334" s="12"/>
     </row>
     <row r="335" ht="14.25" customHeight="1">
       <c r="W335" s="12"/>
@@ -15526,7 +15550,9 @@
     <row r="391" ht="14.25" customHeight="1">
       <c r="W391" s="12"/>
     </row>
-    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="392" ht="14.25" customHeight="1">
+      <c r="W392" s="12"/>
+    </row>
     <row r="393" ht="15.75" customHeight="1"/>
     <row r="394" ht="15.75" customHeight="1"/>
     <row r="395" ht="15.75" customHeight="1"/>
@@ -16136,15 +16162,10 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="$A$9:$W$191">
+  <autoFilter ref="$A$9:$W$192">
     <filterColumn colId="2">
       <filters>
         <filter val="RAP"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="22">
-      <filters>
-        <filter val="KO"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -16158,14 +16179,23 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K10:K180">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K148:K163">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T148:T163">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J10:J147 M10:N147 P10:R147 J163:J192 M164:N192 P164:R192">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K10:K147 K164:K192">
       <formula1>'LISTA VALORI'!$A$2:$A$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T10:T12 T14 T16:T20 T22 T24:T28 T30:T180">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T10:T147 T164:T192">
       <formula1>Sheet1!$A$2:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J10:J12 M10:N12 P10:R12 J14 M14:N14 P14:R14 J16:J20 M16:N20 P16:R20 J22 M22:N22 P22:R22 J24:J28 M24:N28 P24:R28 J30:J164 J166:J180 M30:N180 P30:R180">
-      <formula1>Sheet1!$B$2:$B$3</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J148:J162 M148:N163 P148:R163">
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>
@@ -16190,43 +16220,43 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="48" t="s">
-        <v>440</v>
+      <c r="A1" s="55" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="48" t="s">
-        <v>441</v>
+      <c r="A2" s="55" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="48" t="s">
-        <v>373</v>
+      <c r="A3" s="55" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="48" t="s">
-        <v>442</v>
+      <c r="A4" s="55" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="48" t="s">
-        <v>382</v>
+      <c r="A5" s="55" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="48" t="s">
-        <v>443</v>
+      <c r="A6" s="55" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="48" t="s">
-        <v>363</v>
+      <c r="A7" s="55" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="48" t="s">
-        <v>444</v>
+      <c r="A8" s="55" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1"/>
@@ -17252,163 +17282,163 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="49" t="s">
-        <v>445</v>
-      </c>
-      <c r="B1" s="50" t="s">
+      <c r="A1" s="56" t="s">
+        <v>447</v>
+      </c>
+      <c r="B1" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="50" t="s">
-        <v>446</v>
-      </c>
-      <c r="D1" s="50" t="s">
-        <v>447</v>
-      </c>
-      <c r="F1" s="51" t="s">
+      <c r="C1" s="57" t="s">
         <v>448</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="D1" s="57" t="s">
         <v>449</v>
       </c>
+      <c r="F1" s="58" t="s">
+        <v>450</v>
+      </c>
+      <c r="G1" s="59" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="53" t="s">
-        <v>450</v>
-      </c>
-      <c r="C2" s="54" t="s">
-        <v>451</v>
-      </c>
-      <c r="D2" s="54" t="s">
+      <c r="B2" s="60" t="s">
         <v>452</v>
       </c>
+      <c r="C2" s="61" t="s">
+        <v>453</v>
+      </c>
+      <c r="D2" s="61" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="53" t="s">
-        <v>450</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>453</v>
-      </c>
-      <c r="D3" s="54" t="s">
-        <v>454</v>
+      <c r="B3" s="60" t="s">
+        <v>452</v>
+      </c>
+      <c r="C3" s="61" t="s">
+        <v>455</v>
+      </c>
+      <c r="D3" s="61" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="53" t="s">
-        <v>450</v>
-      </c>
-      <c r="C4" s="54">
-        <v>446.447</v>
-      </c>
-      <c r="D4" s="55" t="s">
-        <v>455</v>
+      <c r="B4" s="60" t="s">
+        <v>452</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>457</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="53" t="s">
-        <v>450</v>
-      </c>
-      <c r="C5" s="54" t="s">
-        <v>456</v>
-      </c>
-      <c r="D5" s="54" t="s">
-        <v>457</v>
+      <c r="B5" s="60" t="s">
+        <v>452</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>459</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="53" t="s">
-        <v>450</v>
-      </c>
-      <c r="C6" s="54" t="s">
-        <v>458</v>
-      </c>
-      <c r="D6" s="55" t="s">
-        <v>459</v>
+      <c r="B6" s="60" t="s">
+        <v>452</v>
+      </c>
+      <c r="C6" s="61" t="s">
+        <v>461</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="53" t="s">
-        <v>450</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>460</v>
-      </c>
-      <c r="D7" s="55" t="s">
-        <v>461</v>
+      <c r="B7" s="60" t="s">
+        <v>452</v>
+      </c>
+      <c r="C7" s="61" t="s">
+        <v>463</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="53" t="s">
-        <v>450</v>
-      </c>
-      <c r="C8" s="54" t="s">
-        <v>462</v>
-      </c>
-      <c r="D8" s="55" t="s">
-        <v>463</v>
+      <c r="B8" s="60" t="s">
+        <v>452</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>465</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="53" t="s">
-        <v>450</v>
-      </c>
-      <c r="C9" s="54" t="s">
-        <v>464</v>
-      </c>
-      <c r="D9" s="55" t="s">
-        <v>465</v>
+      <c r="B9" s="60" t="s">
+        <v>452</v>
+      </c>
+      <c r="C9" s="61" t="s">
+        <v>467</v>
+      </c>
+      <c r="D9" s="62" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="53" t="s">
-        <v>466</v>
-      </c>
-      <c r="B10" s="53" t="s">
-        <v>450</v>
-      </c>
-      <c r="C10" s="55" t="s">
-        <v>467</v>
-      </c>
-      <c r="D10" s="54" t="s">
-        <v>468</v>
+      <c r="A10" s="60" t="s">
+        <v>469</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>452</v>
+      </c>
+      <c r="C10" s="62" t="s">
+        <v>470</v>
+      </c>
+      <c r="D10" s="61" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="53" t="s">
-        <v>331</v>
-      </c>
-      <c r="B11" s="53" t="s">
-        <v>450</v>
-      </c>
-      <c r="C11" s="54" t="s">
-        <v>469</v>
-      </c>
-      <c r="D11" s="55" t="s">
-        <v>470</v>
+      <c r="A11" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>452</v>
+      </c>
+      <c r="C11" s="61" t="s">
+        <v>472</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
@@ -20405,27 +20435,27 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="63" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="56" t="s">
-        <v>336</v>
-      </c>
-      <c r="B2" s="56" t="s">
+      <c r="A2" s="63" t="s">
+        <v>332</v>
+      </c>
+      <c r="B2" s="63" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="56" t="s">
-        <v>353</v>
-      </c>
-      <c r="B3" s="56" t="s">
-        <v>347</v>
+      <c r="A3" s="63" t="s">
+        <v>349</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Aggiornato il file report
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-RAP/V.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-RAP/V.2.0/report-checklist.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="472">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1974,12 +1974,6 @@
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt avente dei campi valorizzati in maniera errata al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 Al fine di rendere non valido il token è necessario valorizzare il campo "action_id" con la stringa "TEST" (valore non ammesso).</t>
     </r>
-  </si>
-  <si>
-    <t>7c8e659369f8b15550558c85c6f40188</t>
-  </si>
-  <si>
-    <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
     <t>Campo/sezione non gestito/a in modo strutturato dall’applicativo</t>
@@ -2748,7 +2742,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2863,9 +2857,6 @@
     </xf>
     <xf borderId="22" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="23" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -10939,29 +10930,21 @@
       <c r="E152" s="35" t="s">
         <v>347</v>
       </c>
-      <c r="F152" s="37">
-        <v>45805.0</v>
-      </c>
-      <c r="G152" s="43">
-        <v>1.748435747E12</v>
-      </c>
-      <c r="H152" s="43" t="s">
+      <c r="F152" s="37"/>
+      <c r="G152" s="43"/>
+      <c r="H152" s="43"/>
+      <c r="I152" s="44"/>
+      <c r="J152" s="38" t="s">
+        <v>344</v>
+      </c>
+      <c r="K152" s="38" t="s">
         <v>348</v>
-      </c>
-      <c r="I152" s="44" t="s">
-        <v>349</v>
-      </c>
-      <c r="J152" s="45" t="s">
-        <v>344</v>
-      </c>
-      <c r="K152" s="45" t="s">
-        <v>350</v>
       </c>
       <c r="L152" s="38"/>
       <c r="M152" s="38"/>
       <c r="N152" s="38"/>
       <c r="O152" s="38" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="P152" s="38"/>
       <c r="Q152" s="38"/>
@@ -10985,10 +10968,10 @@
         <v>328</v>
       </c>
       <c r="D153" s="34" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E153" s="35" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F153" s="37"/>
       <c r="G153" s="37"/>
@@ -11001,7 +10984,7 @@
         <v>345</v>
       </c>
       <c r="L153" s="38"/>
-      <c r="M153" s="45" t="s">
+      <c r="M153" s="38" t="s">
         <v>344</v>
       </c>
       <c r="N153" s="38" t="s">
@@ -11038,10 +11021,10 @@
         <v>328</v>
       </c>
       <c r="D154" s="34" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E154" s="35" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F154" s="37">
         <v>45805.0</v>
@@ -11050,10 +11033,10 @@
         <v>1.748434847E12</v>
       </c>
       <c r="H154" s="43" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="I154" s="44" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="J154" s="38" t="s">
         <v>94</v>
@@ -11067,7 +11050,7 @@
         <v>344</v>
       </c>
       <c r="O154" s="38" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="P154" s="38" t="s">
         <v>94</v>
@@ -11078,7 +11061,7 @@
       <c r="R154" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="S154" s="45" t="s">
+      <c r="S154" s="38" t="s">
         <v>344</v>
       </c>
       <c r="T154" s="38"/>
@@ -11099,10 +11082,10 @@
         <v>328</v>
       </c>
       <c r="D155" s="34" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E155" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F155" s="37"/>
       <c r="G155" s="37"/>
@@ -11140,10 +11123,10 @@
         <v>328</v>
       </c>
       <c r="D156" s="34" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E156" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F156" s="37"/>
       <c r="G156" s="37"/>
@@ -11153,7 +11136,7 @@
         <v>344</v>
       </c>
       <c r="K156" s="38" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L156" s="38"/>
       <c r="M156" s="38"/>
@@ -11181,10 +11164,10 @@
         <v>328</v>
       </c>
       <c r="D157" s="34" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E157" s="35" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F157" s="37">
         <v>45805.0</v>
@@ -11193,10 +11176,10 @@
         <v>1.748438752E12</v>
       </c>
       <c r="H157" s="43" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I157" s="44" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="J157" s="38" t="s">
         <v>94</v>
@@ -11210,18 +11193,18 @@
         <v>344</v>
       </c>
       <c r="O157" s="38" t="s">
-        <v>368</v>
-      </c>
-      <c r="P157" s="45" t="s">
+        <v>366</v>
+      </c>
+      <c r="P157" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="Q157" s="45" t="s">
+      <c r="Q157" s="38" t="s">
         <v>344</v>
       </c>
-      <c r="R157" s="45" t="s">
+      <c r="R157" s="38" t="s">
         <v>344</v>
       </c>
-      <c r="S157" s="45" t="s">
+      <c r="S157" s="38" t="s">
         <v>344</v>
       </c>
       <c r="T157" s="38"/>
@@ -11242,10 +11225,10 @@
         <v>328</v>
       </c>
       <c r="D158" s="34" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E158" s="35" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F158" s="37"/>
       <c r="G158" s="37"/>
@@ -11255,7 +11238,7 @@
         <v>344</v>
       </c>
       <c r="K158" s="38" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L158" s="38"/>
       <c r="M158" s="38"/>
@@ -11283,10 +11266,10 @@
         <v>328</v>
       </c>
       <c r="D159" s="34" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E159" s="35" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F159" s="37"/>
       <c r="G159" s="37"/>
@@ -11296,7 +11279,7 @@
         <v>344</v>
       </c>
       <c r="K159" s="38" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L159" s="38"/>
       <c r="M159" s="38"/>
@@ -11324,10 +11307,10 @@
         <v>328</v>
       </c>
       <c r="D160" s="34" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E160" s="35" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F160" s="37"/>
       <c r="G160" s="37"/>
@@ -11337,7 +11320,7 @@
         <v>344</v>
       </c>
       <c r="K160" s="38" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L160" s="38"/>
       <c r="M160" s="38"/>
@@ -11365,10 +11348,10 @@
         <v>328</v>
       </c>
       <c r="D161" s="34" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E161" s="35" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F161" s="37"/>
       <c r="G161" s="37"/>
@@ -11378,7 +11361,7 @@
         <v>344</v>
       </c>
       <c r="K161" s="38" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L161" s="38"/>
       <c r="M161" s="38"/>
@@ -11406,10 +11389,10 @@
         <v>328</v>
       </c>
       <c r="D162" s="34" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E162" s="35" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F162" s="37"/>
       <c r="G162" s="37"/>
@@ -11419,7 +11402,7 @@
         <v>344</v>
       </c>
       <c r="K162" s="38" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L162" s="38"/>
       <c r="M162" s="38"/>
@@ -11447,10 +11430,10 @@
         <v>328</v>
       </c>
       <c r="D163" s="34" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E163" s="35" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F163" s="37"/>
       <c r="G163" s="37"/>
@@ -11460,7 +11443,7 @@
         <v>344</v>
       </c>
       <c r="K163" s="38" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L163" s="38"/>
       <c r="M163" s="38"/>
@@ -11488,10 +11471,10 @@
         <v>58</v>
       </c>
       <c r="D164" s="34" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E164" s="35" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F164" s="37"/>
       <c r="G164" s="37"/>
@@ -11525,10 +11508,10 @@
         <v>58</v>
       </c>
       <c r="D165" s="34" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E165" s="35" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F165" s="37"/>
       <c r="G165" s="37"/>
@@ -11562,10 +11545,10 @@
         <v>64</v>
       </c>
       <c r="D166" s="34" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E166" s="35" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F166" s="37"/>
       <c r="G166" s="37"/>
@@ -11599,10 +11582,10 @@
         <v>64</v>
       </c>
       <c r="D167" s="34" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E167" s="35" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F167" s="37"/>
       <c r="G167" s="37"/>
@@ -11636,10 +11619,10 @@
         <v>55</v>
       </c>
       <c r="D168" s="34" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E168" s="35" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F168" s="37"/>
       <c r="G168" s="37"/>
@@ -11673,10 +11656,10 @@
         <v>55</v>
       </c>
       <c r="D169" s="34" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E169" s="35" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F169" s="37"/>
       <c r="G169" s="37"/>
@@ -11710,10 +11693,10 @@
         <v>48</v>
       </c>
       <c r="D170" s="34" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E170" s="35" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F170" s="37"/>
       <c r="G170" s="37"/>
@@ -11747,10 +11730,10 @@
         <v>73</v>
       </c>
       <c r="D171" s="34" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E171" s="35" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F171" s="37"/>
       <c r="G171" s="37"/>
@@ -11784,10 +11767,10 @@
         <v>73</v>
       </c>
       <c r="D172" s="34" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E172" s="35" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F172" s="37"/>
       <c r="G172" s="37"/>
@@ -11821,10 +11804,10 @@
         <v>70</v>
       </c>
       <c r="D173" s="34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E173" s="35" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F173" s="37"/>
       <c r="G173" s="37"/>
@@ -11858,10 +11841,10 @@
         <v>70</v>
       </c>
       <c r="D174" s="34" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E174" s="35" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F174" s="37"/>
       <c r="G174" s="37"/>
@@ -11895,10 +11878,10 @@
         <v>67</v>
       </c>
       <c r="D175" s="34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E175" s="35" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F175" s="37"/>
       <c r="G175" s="37"/>
@@ -11932,10 +11915,10 @@
         <v>67</v>
       </c>
       <c r="D176" s="34" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E176" s="35" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F176" s="37"/>
       <c r="G176" s="37"/>
@@ -11969,10 +11952,10 @@
         <v>328</v>
       </c>
       <c r="D177" s="34" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E177" s="35" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F177" s="37">
         <v>45805.0</v>
@@ -11981,10 +11964,10 @@
         <v>1.748428967E12</v>
       </c>
       <c r="H177" s="43" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I177" s="44" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="J177" s="38" t="s">
         <v>94</v>
@@ -12018,10 +12001,10 @@
         <v>64</v>
       </c>
       <c r="D178" s="34" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E178" s="35" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F178" s="34"/>
       <c r="G178" s="34"/>
@@ -12055,10 +12038,10 @@
         <v>61</v>
       </c>
       <c r="D179" s="34" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E179" s="35" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F179" s="34"/>
       <c r="G179" s="34"/>
@@ -12092,10 +12075,10 @@
         <v>73</v>
       </c>
       <c r="D180" s="34" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E180" s="35" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F180" s="34"/>
       <c r="G180" s="34"/>
@@ -12129,10 +12112,10 @@
         <v>67</v>
       </c>
       <c r="D181" s="34" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E181" s="35" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F181" s="34"/>
       <c r="G181" s="34"/>
@@ -12166,10 +12149,10 @@
         <v>70</v>
       </c>
       <c r="D182" s="34" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E182" s="35" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F182" s="34"/>
       <c r="G182" s="34"/>
@@ -12203,10 +12186,10 @@
         <v>48</v>
       </c>
       <c r="D183" s="34" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E183" s="35" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F183" s="34"/>
       <c r="G183" s="34"/>
@@ -12240,10 +12223,10 @@
         <v>55</v>
       </c>
       <c r="D184" s="34" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E184" s="35" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F184" s="34"/>
       <c r="G184" s="34"/>
@@ -12277,10 +12260,10 @@
         <v>64</v>
       </c>
       <c r="D185" s="34" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E185" s="35" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F185" s="34"/>
       <c r="G185" s="34"/>
@@ -12314,10 +12297,10 @@
         <v>58</v>
       </c>
       <c r="D186" s="34" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E186" s="35" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F186" s="34"/>
       <c r="G186" s="34"/>
@@ -12351,10 +12334,10 @@
         <v>328</v>
       </c>
       <c r="D187" s="34" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E187" s="35" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F187" s="34"/>
       <c r="G187" s="34"/>
@@ -12364,7 +12347,7 @@
         <v>344</v>
       </c>
       <c r="K187" s="38" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L187" s="34"/>
       <c r="M187" s="38"/>
@@ -12392,10 +12375,10 @@
         <v>61</v>
       </c>
       <c r="D188" s="34" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E188" s="35" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F188" s="37"/>
       <c r="G188" s="37"/>
@@ -12429,10 +12412,10 @@
         <v>61</v>
       </c>
       <c r="D189" s="34" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E189" s="35" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F189" s="37"/>
       <c r="G189" s="37"/>
@@ -12466,10 +12449,10 @@
         <v>48</v>
       </c>
       <c r="D190" s="41" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E190" s="35" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F190" s="37"/>
       <c r="G190" s="37"/>
@@ -12503,10 +12486,10 @@
         <v>61</v>
       </c>
       <c r="D191" s="34" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E191" s="35" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F191" s="37"/>
       <c r="G191" s="37"/>
@@ -12540,10 +12523,10 @@
         <v>64</v>
       </c>
       <c r="D192" s="34" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E192" s="35" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F192" s="37"/>
       <c r="G192" s="37"/>
@@ -16138,14 +16121,14 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J10:J192 M10:N192 P10:R192">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T10:T192">
       <formula1>Sheet1!$A$2:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K10:K192">
       <formula1>'LISTA VALORI'!$A$2:$A$8</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J10:J192 M10:N192 P10:R192">
-      <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>
@@ -16170,43 +16153,43 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="45" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="45" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="45" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="45" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="45" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" s="45" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="46" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="46" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="46" t="s">
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" s="45" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25" customHeight="1">
+      <c r="A8" s="45" t="s">
         <v>443</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="46" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="46" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="46" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="46" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1"/>
@@ -17232,163 +17215,163 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
+        <v>444</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>445</v>
+      </c>
+      <c r="D1" s="47" t="s">
         <v>446</v>
       </c>
-      <c r="B1" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="48" t="s">
+      <c r="F1" s="48" t="s">
         <v>447</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="G1" s="49" t="s">
         <v>448</v>
       </c>
-      <c r="F1" s="49" t="s">
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="50" t="s">
         <v>449</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="C2" s="51" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="51" t="s">
+      <c r="D2" s="51" t="s">
         <v>451</v>
       </c>
-      <c r="C2" s="52" t="s">
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>449</v>
+      </c>
+      <c r="C3" s="51" t="s">
         <v>452</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D3" s="51" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="51" t="s">
-        <v>451</v>
-      </c>
-      <c r="C3" s="52" t="s">
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>449</v>
+      </c>
+      <c r="C4" s="51" t="s">
         <v>454</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D4" s="52" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="51" t="s">
-        <v>451</v>
-      </c>
-      <c r="C4" s="52" t="s">
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>449</v>
+      </c>
+      <c r="C5" s="51" t="s">
         <v>456</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D5" s="51" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="51" t="s">
-        <v>451</v>
-      </c>
-      <c r="C5" s="52" t="s">
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>449</v>
+      </c>
+      <c r="C6" s="51" t="s">
         <v>458</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D6" s="52" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="51" t="s">
-        <v>451</v>
-      </c>
-      <c r="C6" s="52" t="s">
+    <row r="7">
+      <c r="A7" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>449</v>
+      </c>
+      <c r="C7" s="51" t="s">
         <v>460</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D7" s="52" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="51" t="s">
-        <v>451</v>
-      </c>
-      <c r="C7" s="52" t="s">
+    <row r="8">
+      <c r="A8" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>449</v>
+      </c>
+      <c r="C8" s="51" t="s">
         <v>462</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D8" s="52" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="51" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="51" t="s">
-        <v>451</v>
-      </c>
-      <c r="C8" s="52" t="s">
+    <row r="9">
+      <c r="A9" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>449</v>
+      </c>
+      <c r="C9" s="51" t="s">
         <v>464</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D9" s="52" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="51" t="s">
-        <v>451</v>
-      </c>
-      <c r="C9" s="52" t="s">
+    <row r="10">
+      <c r="A10" s="50" t="s">
         <v>466</v>
       </c>
-      <c r="D9" s="53" t="s">
+      <c r="B10" s="50" t="s">
+        <v>449</v>
+      </c>
+      <c r="C10" s="52" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="51" t="s">
+      <c r="D10" s="51" t="s">
         <v>468</v>
       </c>
-      <c r="B10" s="51" t="s">
-        <v>451</v>
-      </c>
-      <c r="C10" s="53" t="s">
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" s="50" t="s">
+        <v>328</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>449</v>
+      </c>
+      <c r="C11" s="51" t="s">
         <v>469</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D11" s="52" t="s">
         <v>470</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="51" t="s">
-        <v>328</v>
-      </c>
-      <c r="B11" s="51" t="s">
-        <v>451</v>
-      </c>
-      <c r="C11" s="52" t="s">
-        <v>471</v>
-      </c>
-      <c r="D11" s="53" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
@@ -18825,26 +18808,26 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="53" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>333</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="53" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="54" t="s">
-        <v>473</v>
-      </c>
-      <c r="B3" s="54" t="s">
+      <c r="A3" s="53" t="s">
+        <v>471</v>
+      </c>
+      <c r="B3" s="53" t="s">
         <v>344</v>
       </c>
     </row>

</xml_diff>